<commit_message>
Fixing errors in filtering log data
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2018/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53616140-ABF6-6D40-8BDB-F5FEA4F837F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73F2B06-12FF-D84A-9BCB-6F409610C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="160">
   <si>
     <t>Collection Day</t>
   </si>
@@ -512,6 +512,12 @@
   </si>
   <si>
     <t>F_Sed_4m_R2_F8_25Jun18</t>
+  </si>
+  <si>
+    <t>F_Sed_4m_R2_F4_16Jul18</t>
+  </si>
+  <si>
+    <t>F_Sed_8m_R2_F4_23Jul18</t>
   </si>
 </sst>
 </file>
@@ -534,12 +540,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -569,12 +581,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,19 +906,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J112" sqref="J112:J115"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="25.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="20" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
     <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2818,8 +2833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2517B6EF-0E7C-2942-A10C-608706273F55}">
   <dimension ref="A1:I115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H115"/>
+    <sheetView topLeftCell="B97" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I111" sqref="I111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3437,7 +3452,7 @@
       <c r="G27">
         <v>0.16422</v>
       </c>
-      <c r="H27" s="2" t="s">
+      <c r="H27" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -3713,8 +3728,8 @@
       <c r="G39">
         <v>0.15931999999999999</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>42</v>
+      <c r="H39" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -3814,8 +3829,8 @@
       <c r="G43">
         <v>0.16027</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>38</v>
+      <c r="H43" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
@@ -3932,7 +3947,7 @@
       <c r="G48">
         <v>0.16372</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3955,7 +3970,7 @@
       <c r="G49">
         <v>0.16352</v>
       </c>
-      <c r="H49" s="2" t="s">
+      <c r="H49" s="5" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4116,7 +4131,7 @@
       <c r="G56">
         <v>0.16739999999999999</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4139,7 +4154,7 @@
       <c r="G57">
         <v>0.10548</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4460,7 +4475,7 @@
       <c r="H72" t="s">
         <v>101</v>
       </c>
-      <c r="I72" t="s">
+      <c r="I72" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5178,7 +5193,7 @@
       <c r="H104" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="I104" t="s">
+      <c r="I104" s="7" t="s">
         <v>72</v>
       </c>
     </row>
@@ -5201,7 +5216,7 @@
       <c r="H105" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="I105" t="s">
+      <c r="I105" s="7" t="s">
         <v>73</v>
       </c>
     </row>
@@ -5224,7 +5239,7 @@
       <c r="H106" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="I106" t="s">
+      <c r="I106" s="7" t="s">
         <v>74</v>
       </c>
     </row>
@@ -5247,7 +5262,7 @@
       <c r="H107" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I107" t="s">
+      <c r="I107" s="7" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixing more filtering log errors
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/Virginia Tech/Sed Traps/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73F2B06-12FF-D84A-9BCB-6F409610C994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582640C9-D348-9543-81BC-11E86EC866C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="159">
   <si>
     <t>Collection Day</t>
   </si>
@@ -154,9 +154,6 @@
     <t>F_Sed_8m_R2_F3_23Jul18</t>
   </si>
   <si>
-    <t>F_Sed_8m_R3_F4_23Jul18</t>
-  </si>
-  <si>
     <t>F_Sed_4m_R1_F1_16Jul18</t>
   </si>
   <si>
@@ -166,9 +163,6 @@
     <t>F_Sed_4m_R2_F3_16Jul18</t>
   </si>
   <si>
-    <t>F_Sed_4m_R3_F4_16Jul18</t>
-  </si>
-  <si>
     <t>F_Sed_8m_R1_F1_13Aug18</t>
   </si>
   <si>
@@ -518,6 +512,9 @@
   </si>
   <si>
     <t>F_Sed_8m_R2_F4_23Jul18</t>
+  </si>
+  <si>
+    <t>F_Sed_8m_R2_F4_09Jul18</t>
   </si>
 </sst>
 </file>
@@ -581,14 +578,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -906,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
   <dimension ref="A1:K115"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -925,34 +921,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" t="s">
         <v>85</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J1" t="s">
-        <v>87</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>7</v>
@@ -960,7 +956,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E2">
         <v>0.15815000000000001</v>
@@ -1106,7 +1102,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E12">
         <v>0.16142999999999999</v>
@@ -1123,7 +1119,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13">
         <v>0.16051000000000001</v>
@@ -1140,7 +1136,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E14">
         <v>0.1585</v>
@@ -1157,7 +1153,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E15">
         <v>0.15845999999999999</v>
@@ -1174,7 +1170,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E16">
         <v>0.15742</v>
@@ -1191,7 +1187,7 @@
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E17">
         <v>0.156</v>
@@ -1208,7 +1204,7 @@
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E18">
         <v>0.15608</v>
@@ -1228,7 +1224,7 @@
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E19">
         <v>0.15659999999999999</v>
@@ -1248,7 +1244,7 @@
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E20">
         <v>0.15604999999999999</v>
@@ -1265,7 +1261,7 @@
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E21">
         <v>0.15558</v>
@@ -1282,7 +1278,7 @@
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E22">
         <v>0.15573999999999999</v>
@@ -1299,7 +1295,7 @@
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E23">
         <v>0.15884000000000001</v>
@@ -1316,7 +1312,7 @@
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E24">
         <v>0.15834000000000001</v>
@@ -1333,7 +1329,7 @@
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E25">
         <v>0.15851000000000001</v>
@@ -1350,7 +1346,7 @@
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E26">
         <v>0.15726999999999999</v>
@@ -1367,7 +1363,7 @@
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E27">
         <v>0.15858</v>
@@ -1452,7 +1448,7 @@
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E32">
         <v>0.15787999999999999</v>
@@ -1469,7 +1465,7 @@
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E33">
         <v>0.15583</v>
@@ -1486,7 +1482,7 @@
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E34">
         <v>0.16031000000000001</v>
@@ -1503,7 +1499,7 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="E35">
         <v>0.159</v>
@@ -1520,7 +1516,7 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E36">
         <v>0.15572</v>
@@ -1537,7 +1533,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E37">
         <v>0.15558</v>
@@ -1554,7 +1550,7 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38">
         <v>0.15495</v>
@@ -1571,7 +1567,7 @@
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>42</v>
+        <v>156</v>
       </c>
       <c r="E39">
         <v>0.15687999999999999</v>
@@ -1648,7 +1644,7 @@
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="E43">
         <v>0.15362000000000001</v>
@@ -1668,7 +1664,7 @@
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E44">
         <v>0.15822</v>
@@ -1685,7 +1681,7 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E45">
         <v>0.1575</v>
@@ -1702,7 +1698,7 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E46">
         <v>0.15890000000000001</v>
@@ -1719,7 +1715,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E47">
         <v>0.15909000000000001</v>
@@ -1736,7 +1732,7 @@
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E48">
         <v>0.16075999999999999</v>
@@ -1753,7 +1749,7 @@
     </row>
     <row r="49" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E49">
         <v>0.15915000000000001</v>
@@ -1770,7 +1766,7 @@
     </row>
     <row r="50" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E50">
         <v>0.15617</v>
@@ -1787,7 +1783,7 @@
     </row>
     <row r="51" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E51">
         <v>0.16111</v>
@@ -1804,7 +1800,7 @@
     </row>
     <row r="52" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E52">
         <v>0.16162000000000001</v>
@@ -1821,7 +1817,7 @@
     </row>
     <row r="53" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E53">
         <v>0.156</v>
@@ -1838,7 +1834,7 @@
     </row>
     <row r="54" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E54">
         <v>0.15751999999999999</v>
@@ -1855,7 +1851,7 @@
     </row>
     <row r="55" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E55">
         <v>0.15764</v>
@@ -1872,7 +1868,7 @@
     </row>
     <row r="56" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E56">
         <v>0.16083</v>
@@ -1889,7 +1885,7 @@
     </row>
     <row r="57" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E57">
         <v>0.15933</v>
@@ -1906,7 +1902,7 @@
     </row>
     <row r="58" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C58" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E58">
         <v>0.15851000000000001</v>
@@ -1923,7 +1919,7 @@
     </row>
     <row r="59" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C59" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E59">
         <v>0.15859999999999999</v>
@@ -1946,7 +1942,7 @@
         <v>50</v>
       </c>
       <c r="K60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="3:11" x14ac:dyDescent="0.2">
@@ -1957,7 +1953,7 @@
         <v>55</v>
       </c>
       <c r="K61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="3:11" x14ac:dyDescent="0.2">
@@ -1968,7 +1964,7 @@
         <v>50</v>
       </c>
       <c r="K62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="3:11" x14ac:dyDescent="0.2">
@@ -1979,7 +1975,7 @@
         <v>50</v>
       </c>
       <c r="K63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="3:11" x14ac:dyDescent="0.2">
@@ -1990,7 +1986,7 @@
         <v>50</v>
       </c>
       <c r="K64" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="3:11" x14ac:dyDescent="0.2">
@@ -2001,7 +1997,7 @@
         <v>50</v>
       </c>
       <c r="K65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="3:11" x14ac:dyDescent="0.2">
@@ -2012,7 +2008,7 @@
         <v>75</v>
       </c>
       <c r="K66" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="3:11" x14ac:dyDescent="0.2">
@@ -2023,12 +2019,12 @@
         <v>55</v>
       </c>
       <c r="K67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E68">
         <v>0.15584999999999999</v>
@@ -2045,7 +2041,7 @@
     </row>
     <row r="69" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E69">
         <v>0.15423000000000001</v>
@@ -2062,7 +2058,7 @@
     </row>
     <row r="70" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E70">
         <v>0.15583</v>
@@ -2079,7 +2075,7 @@
     </row>
     <row r="71" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E71">
         <v>0.15587999999999999</v>
@@ -2096,7 +2092,7 @@
     </row>
     <row r="72" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E72">
         <v>0.16233</v>
@@ -2108,12 +2104,12 @@
         <v>14</v>
       </c>
       <c r="K72" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E73">
         <v>0.16169</v>
@@ -2130,7 +2126,7 @@
     </row>
     <row r="74" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E74">
         <v>0.15515000000000001</v>
@@ -2147,7 +2143,7 @@
     </row>
     <row r="75" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E75">
         <v>0.15509000000000001</v>
@@ -2164,7 +2160,7 @@
     </row>
     <row r="76" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E76">
         <v>0.15778</v>
@@ -2181,7 +2177,7 @@
     </row>
     <row r="77" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E77">
         <v>0.15565000000000001</v>
@@ -2198,7 +2194,7 @@
     </row>
     <row r="78" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E78">
         <v>0.15804000000000001</v>
@@ -2215,7 +2211,7 @@
     </row>
     <row r="79" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E79">
         <v>0.15684000000000001</v>
@@ -2232,7 +2228,7 @@
     </row>
     <row r="80" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E80">
         <v>0.13755999999999999</v>
@@ -2249,7 +2245,7 @@
     </row>
     <row r="81" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E81">
         <v>0.15445</v>
@@ -2266,7 +2262,7 @@
     </row>
     <row r="82" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E82">
         <v>0.16009000000000001</v>
@@ -2283,7 +2279,7 @@
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E83">
         <v>0.16098999999999999</v>
@@ -2300,7 +2296,7 @@
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E84">
         <v>0.15984999999999999</v>
@@ -2317,7 +2313,7 @@
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E85">
         <v>0.15867000000000001</v>
@@ -2334,7 +2330,7 @@
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E86">
         <v>0.15931000000000001</v>
@@ -2351,7 +2347,7 @@
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E87">
         <v>0.15812999999999999</v>
@@ -2368,7 +2364,7 @@
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E88">
         <v>0.15898999999999999</v>
@@ -2385,7 +2381,7 @@
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E89">
         <v>0.16089000000000001</v>
@@ -2399,7 +2395,7 @@
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E90">
         <v>0.16186</v>
@@ -2413,7 +2409,7 @@
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E91">
         <v>0.16017000000000001</v>
@@ -2430,7 +2426,7 @@
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E92">
         <v>0.15820000000000001</v>
@@ -2444,7 +2440,7 @@
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E93">
         <v>0.15794</v>
@@ -2458,7 +2454,7 @@
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E94">
         <v>0.15837999999999999</v>
@@ -2472,7 +2468,7 @@
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E95">
         <v>0.15840000000000001</v>
@@ -2486,7 +2482,7 @@
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E96">
         <v>0.15612999999999999</v>
@@ -2503,7 +2499,7 @@
     </row>
     <row r="97" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E97">
         <v>0.13650000000000001</v>
@@ -2520,7 +2516,7 @@
     </row>
     <row r="98" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E98">
         <v>0.15742</v>
@@ -2537,7 +2533,7 @@
     </row>
     <row r="99" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E99">
         <v>0.15698000000000001</v>
@@ -2554,7 +2550,7 @@
     </row>
     <row r="100" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E100">
         <v>0.15665999999999999</v>
@@ -2571,7 +2567,7 @@
     </row>
     <row r="101" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E101">
         <v>0.15712999999999999</v>
@@ -2588,7 +2584,7 @@
     </row>
     <row r="102" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E102">
         <v>0.1573</v>
@@ -2605,7 +2601,7 @@
     </row>
     <row r="103" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C103" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E103">
         <v>0.15776999999999999</v>
@@ -2622,7 +2618,7 @@
     </row>
     <row r="104" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F104">
         <v>0.16849</v>
@@ -2634,12 +2630,12 @@
         <v>42</v>
       </c>
       <c r="K104" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F105">
         <v>0.16799</v>
@@ -2651,12 +2647,12 @@
         <v>42</v>
       </c>
       <c r="K105" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C106" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F106">
         <v>0.16767000000000001</v>
@@ -2668,12 +2664,12 @@
         <v>42</v>
       </c>
       <c r="K106" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C107" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F107">
         <v>0.1663</v>
@@ -2685,12 +2681,12 @@
         <v>42</v>
       </c>
       <c r="K107" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C108" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E108">
         <v>0.15523000000000001</v>
@@ -2707,7 +2703,7 @@
     </row>
     <row r="109" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C109" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E109">
         <v>0.15554000000000001</v>
@@ -2724,7 +2720,7 @@
     </row>
     <row r="110" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C110" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E110">
         <v>0.15518000000000001</v>
@@ -2741,7 +2737,7 @@
     </row>
     <row r="111" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C111" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E111">
         <v>0.15368000000000001</v>
@@ -2758,7 +2754,7 @@
     </row>
     <row r="112" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C112" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E112">
         <v>0.15484000000000001</v>
@@ -2775,7 +2771,7 @@
     </row>
     <row r="113" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C113" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E113">
         <v>0.15522</v>
@@ -2792,7 +2788,7 @@
     </row>
     <row r="114" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C114" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E114">
         <v>0.15653</v>
@@ -2809,7 +2805,7 @@
     </row>
     <row r="115" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C115" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E115">
         <v>0.15406</v>
@@ -2849,7 +2845,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -2878,7 +2874,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1">
         <v>43241</v>
@@ -2896,12 +2892,12 @@
         <v>0.16936999999999999</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1">
         <v>43241</v>
@@ -2924,7 +2920,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1">
         <v>43241</v>
@@ -2935,7 +2931,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1">
         <v>43241</v>
@@ -2958,7 +2954,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1">
         <v>43241</v>
@@ -2981,7 +2977,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1">
         <v>43241</v>
@@ -2992,7 +2988,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1">
         <v>43248</v>
@@ -3015,7 +3011,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B9" s="1">
         <v>43248</v>
@@ -3038,7 +3034,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1">
         <v>43248</v>
@@ -3061,7 +3057,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1">
         <v>43248</v>
@@ -3084,7 +3080,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" s="1">
         <v>43255</v>
@@ -3102,12 +3098,12 @@
         <v>0.17385</v>
       </c>
       <c r="H12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="1">
         <v>43255</v>
@@ -3125,12 +3121,12 @@
         <v>0.17383000000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="1">
         <v>43255</v>
@@ -3148,12 +3144,12 @@
         <v>0.16952</v>
       </c>
       <c r="H14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B15" s="1">
         <v>43255</v>
@@ -3171,12 +3167,12 @@
         <v>0.17163</v>
       </c>
       <c r="H15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1">
         <v>43262</v>
@@ -3199,7 +3195,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="1">
         <v>43262</v>
@@ -3222,7 +3218,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B18" s="1">
         <v>43262</v>
@@ -3248,7 +3244,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B19" s="1">
         <v>43262</v>
@@ -3274,7 +3270,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1">
         <v>43276</v>
@@ -3297,7 +3293,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B21" s="1">
         <v>43276</v>
@@ -3320,7 +3316,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1">
         <v>43276</v>
@@ -3343,7 +3339,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B23" s="1">
         <v>43276</v>
@@ -3366,7 +3362,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" s="1">
         <v>43276</v>
@@ -3389,7 +3385,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1">
         <v>43276</v>
@@ -3412,7 +3408,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1">
         <v>43276</v>
@@ -3435,7 +3431,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B27" s="1">
         <v>43276</v>
@@ -3458,7 +3454,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B28" s="1">
         <v>43283</v>
@@ -3481,7 +3477,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1">
         <v>43283</v>
@@ -3504,7 +3500,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1">
         <v>43283</v>
@@ -3527,7 +3523,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1">
         <v>43283</v>
@@ -3550,7 +3546,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B32" s="1">
         <v>43290</v>
@@ -3568,12 +3564,12 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>43290</v>
@@ -3591,12 +3587,12 @@
         <v>0.16569</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B34" s="1">
         <v>43290</v>
@@ -3614,12 +3610,12 @@
         <v>0.16388</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" s="1">
         <v>43290</v>
@@ -3637,12 +3633,12 @@
         <v>0.16339999999999999</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" s="1">
         <v>43297</v>
@@ -3660,12 +3656,12 @@
         <v>0.15801000000000001</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" s="1">
         <v>43297</v>
@@ -3683,12 +3679,12 @@
         <v>0.15790000000000001</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" s="1">
         <v>43297</v>
@@ -3706,12 +3702,12 @@
         <v>0.13771</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" s="1">
         <v>43297</v>
@@ -3728,13 +3724,13 @@
       <c r="G39">
         <v>0.15931999999999999</v>
       </c>
-      <c r="H39" s="6" t="s">
-        <v>158</v>
+      <c r="H39" s="2" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B40" s="1">
         <v>43304</v>
@@ -3760,7 +3756,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1">
         <v>43304</v>
@@ -3786,7 +3782,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B42" s="1">
         <v>43304</v>
@@ -3812,7 +3808,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B43" s="1">
         <v>43304</v>
@@ -3829,8 +3825,8 @@
       <c r="G43">
         <v>0.16027</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>159</v>
+      <c r="H43" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
@@ -3838,7 +3834,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B44" s="1">
         <v>43314</v>
@@ -3856,12 +3852,12 @@
         <v>0.16250000000000001</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B45" s="1">
         <v>43314</v>
@@ -3879,12 +3875,12 @@
         <v>0.16222</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1">
         <v>43314</v>
@@ -3902,12 +3898,12 @@
         <v>0.16397999999999999</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B47" s="1">
         <v>43314</v>
@@ -3925,12 +3921,12 @@
         <v>0.16452</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B48" s="1">
         <v>43325</v>
@@ -3948,12 +3944,12 @@
         <v>0.16372</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B49" s="1">
         <v>43325</v>
@@ -3971,12 +3967,12 @@
         <v>0.16352</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B50" s="1">
         <v>43325</v>
@@ -3994,12 +3990,12 @@
         <v>0.161</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="1">
         <v>43325</v>
@@ -4017,12 +4013,12 @@
         <v>0.16603000000000001</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B52" s="1">
         <v>43332</v>
@@ -4040,12 +4036,12 @@
         <v>0.166603</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B53" s="1">
         <v>43332</v>
@@ -4063,12 +4059,12 @@
         <v>0.1666</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B54" s="1">
         <v>43332</v>
@@ -4086,12 +4082,12 @@
         <v>0.16034999999999999</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B55" s="1">
         <v>43332</v>
@@ -4109,12 +4105,12 @@
         <v>0.16199</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B56" s="1">
         <v>43339</v>
@@ -4132,12 +4128,12 @@
         <v>0.16739999999999999</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B57" s="1">
         <v>43339</v>
@@ -4155,12 +4151,12 @@
         <v>0.10548</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B58" s="1">
         <v>43339</v>
@@ -4178,12 +4174,12 @@
         <v>0.1636</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59" s="1">
         <v>43339</v>
@@ -4201,12 +4197,12 @@
         <v>0.16367000000000001</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60" s="1">
         <v>43336</v>
@@ -4221,12 +4217,12 @@
         <v>0.15726000000000001</v>
       </c>
       <c r="I60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B61" s="1">
         <v>43336</v>
@@ -4241,12 +4237,12 @@
         <v>0.15479999999999999</v>
       </c>
       <c r="I61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B62" s="1">
         <v>43336</v>
@@ -4261,12 +4257,12 @@
         <v>0.15870000000000001</v>
       </c>
       <c r="I62" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B63" s="1">
         <v>43336</v>
@@ -4281,12 +4277,12 @@
         <v>0.15689</v>
       </c>
       <c r="I63" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B64" s="1">
         <v>43336</v>
@@ -4301,12 +4297,12 @@
         <v>0.15905</v>
       </c>
       <c r="I64" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B65" s="1">
         <v>43336</v>
@@ -4321,12 +4317,12 @@
         <v>0.15745000000000001</v>
       </c>
       <c r="I65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B66" s="1">
         <v>43336</v>
@@ -4341,12 +4337,12 @@
         <v>0.15409</v>
       </c>
       <c r="I66" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B67" s="1">
         <v>43336</v>
@@ -4361,12 +4357,12 @@
         <v>0.15523999999999999</v>
       </c>
       <c r="I67" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B68" s="1">
         <v>43346</v>
@@ -4384,12 +4380,12 @@
         <v>0.15847</v>
       </c>
       <c r="H68" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B69" s="1">
         <v>43346</v>
@@ -4407,12 +4403,12 @@
         <v>0.15701999999999999</v>
       </c>
       <c r="H69" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B70" s="1">
         <v>43346</v>
@@ -4430,12 +4426,12 @@
         <v>0.15817999999999999</v>
       </c>
       <c r="H70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B71" s="1">
         <v>43346</v>
@@ -4453,12 +4449,12 @@
         <v>0.15841</v>
       </c>
       <c r="H71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B72" s="1">
         <v>43350</v>
@@ -4473,15 +4469,15 @@
         <v>0.16233</v>
       </c>
       <c r="H72" t="s">
-        <v>101</v>
-      </c>
-      <c r="I72" s="7" t="s">
-        <v>55</v>
+        <v>99</v>
+      </c>
+      <c r="I72" s="6" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B73" s="1">
         <v>43350</v>
@@ -4499,12 +4495,12 @@
         <v>0.16561999999999999</v>
       </c>
       <c r="H73" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B74" s="1">
         <v>43350</v>
@@ -4522,12 +4518,12 @@
         <v>0.15945999999999999</v>
       </c>
       <c r="H74" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B75" s="1">
         <v>43350</v>
@@ -4545,12 +4541,12 @@
         <v>0.15905</v>
       </c>
       <c r="H75" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B76" s="1">
         <v>43350</v>
@@ -4568,12 +4564,12 @@
         <v>0.16339999999999999</v>
       </c>
       <c r="H76" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B77" s="1">
         <v>43350</v>
@@ -4591,12 +4587,12 @@
         <v>0.16034999999999999</v>
       </c>
       <c r="H77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B78" s="1">
         <v>43350</v>
@@ -4614,12 +4610,12 @@
         <v>0.16608999999999999</v>
       </c>
       <c r="H78" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B79" s="1">
         <v>43350</v>
@@ -4637,12 +4633,12 @@
         <v>0.16416</v>
       </c>
       <c r="H79" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B80" s="1">
         <v>43353</v>
@@ -4660,12 +4656,12 @@
         <v>0.17122999999999999</v>
       </c>
       <c r="H80" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B81" s="1">
         <v>43353</v>
@@ -4683,12 +4679,12 @@
         <v>0.16539999999999999</v>
       </c>
       <c r="H81" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B82" s="1">
         <v>43353</v>
@@ -4706,12 +4702,12 @@
         <v>0.16852</v>
       </c>
       <c r="H82" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B83" s="1">
         <v>43353</v>
@@ -4729,12 +4725,12 @@
         <v>0.16628999999999999</v>
       </c>
       <c r="H83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B84" s="1">
         <v>43364</v>
@@ -4752,12 +4748,12 @@
         <v>0.16464000000000001</v>
       </c>
       <c r="H84" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B85" s="1">
         <v>43364</v>
@@ -4775,12 +4771,12 @@
         <v>0.16456999999999999</v>
       </c>
       <c r="H85" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B86" s="1">
         <v>43364</v>
@@ -4798,12 +4794,12 @@
         <v>0.16367000000000001</v>
       </c>
       <c r="H86" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B87" s="1">
         <v>43364</v>
@@ -4821,12 +4817,12 @@
         <v>0.16428999999999999</v>
       </c>
       <c r="H87" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B88" s="1">
         <v>43364</v>
@@ -4844,12 +4840,12 @@
         <v>0.16284999999999999</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B89" s="1">
         <v>43364</v>
@@ -4864,12 +4860,12 @@
         <v>0.16089000000000001</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B90" s="1">
         <v>43364</v>
@@ -4884,12 +4880,12 @@
         <v>0.16186</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B91" s="1">
         <v>43364</v>
@@ -4907,12 +4903,12 @@
         <v>0.16567999999999999</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B92" s="1">
         <v>43378</v>
@@ -4927,12 +4923,12 @@
         <v>0.16291</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B93" s="1">
         <v>43378</v>
@@ -4947,12 +4943,12 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B94" s="1">
         <v>43378</v>
@@ -4967,12 +4963,12 @@
         <v>0.16186</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B95" s="1">
         <v>43378</v>
@@ -4987,12 +4983,12 @@
         <v>0.16184000000000001</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B96" s="1">
         <v>43378</v>
@@ -5010,12 +5006,12 @@
         <v>0.16184000000000001</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B97" s="1">
         <v>43378</v>
@@ -5033,12 +5029,12 @@
         <v>0.16245999999999999</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B98" s="1">
         <v>43378</v>
@@ -5056,12 +5052,12 @@
         <v>0.16263</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B99" s="1">
         <v>43378</v>
@@ -5079,12 +5075,12 @@
         <v>0.16225999999999999</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B100" s="1">
         <v>43381</v>
@@ -5102,12 +5098,12 @@
         <v>0.15956999999999999</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B101" s="1">
         <v>43381</v>
@@ -5125,12 +5121,12 @@
         <v>0.1593</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B102" s="1">
         <v>43381</v>
@@ -5148,12 +5144,12 @@
         <v>0.15947</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B103" s="1">
         <v>43381</v>
@@ -5171,12 +5167,12 @@
         <v>0.15970999999999999</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B104" s="1">
         <v>43395</v>
@@ -5191,15 +5187,15 @@
         <v>0.16849</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="I104" s="7" t="s">
-        <v>72</v>
+        <v>128</v>
+      </c>
+      <c r="I104" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B105" s="1">
         <v>43395</v>
@@ -5214,15 +5210,15 @@
         <v>0.16799</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="I105" s="7" t="s">
-        <v>73</v>
+        <v>129</v>
+      </c>
+      <c r="I105" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B106" s="3">
         <v>43395</v>
@@ -5237,15 +5233,15 @@
         <v>0.16767000000000001</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="I106" s="7" t="s">
-        <v>74</v>
+        <v>130</v>
+      </c>
+      <c r="I106" s="6" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B107" s="3">
         <v>43395</v>
@@ -5260,15 +5256,15 @@
         <v>0.1663</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I107" s="7" t="s">
-        <v>75</v>
+        <v>131</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B108" s="1">
         <v>43402</v>
@@ -5286,12 +5282,12 @@
         <v>0.16098000000000001</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B109" s="1">
         <v>43402</v>
@@ -5309,12 +5305,12 @@
         <v>0.16142999999999999</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B110" s="1">
         <v>43402</v>
@@ -5332,12 +5328,12 @@
         <v>0.16142999999999999</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B111" s="1">
         <v>43402</v>
@@ -5355,12 +5351,12 @@
         <v>0.15926999999999999</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B112" s="1">
         <v>43402</v>
@@ -5378,12 +5374,12 @@
         <v>0.16116</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B113" s="1">
         <v>43402</v>
@@ -5401,12 +5397,12 @@
         <v>0.16186</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B114" s="1">
         <v>43402</v>
@@ -5424,12 +5420,12 @@
         <v>0.16450000000000001</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B115" s="1">
         <v>43402</v>
@@ -5447,7 +5443,7 @@
         <v>0.16012000000000001</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5467,54 +5463,54 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting 2018 filtering log and acid digestion data
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582640C9-D348-9543-81BC-11E86EC866C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F57357-9FF3-954C-80E3-70F4CC7BF6E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="161">
   <si>
     <t>Collection Day</t>
   </si>
@@ -515,12 +515,21 @@
   </si>
   <si>
     <t>F_Sed_8m_R2_F4_09Jul18</t>
+  </si>
+  <si>
+    <t>B_Sed_4m_R1_F2_07Sep18</t>
+  </si>
+  <si>
+    <t>B_Sed_4m_R1_F3_07Sep18</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -578,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -586,6 +595,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
-  <dimension ref="A1:K115"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -911,7 +922,7 @@
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="20" customWidth="1"/>
@@ -932,7 +943,7 @@
       <c r="D1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="8" t="s">
         <v>80</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -958,7 +969,7 @@
       <c r="C2" t="s">
         <v>86</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>0.15815000000000001</v>
       </c>
       <c r="F2">
@@ -975,7 +986,7 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="7">
         <v>0.16</v>
       </c>
       <c r="F3">
@@ -989,19 +1000,31 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.159</v>
+      </c>
+      <c r="F4">
+        <v>0.17119000000000001</v>
+      </c>
+      <c r="G4">
+        <v>197</v>
+      </c>
       <c r="J4">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>0.159</v>
+        <v>12</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0.15643000000000001</v>
       </c>
       <c r="F5">
-        <v>0.17119000000000001</v>
+        <v>0.16766</v>
       </c>
       <c r="G5">
         <v>197</v>
@@ -1012,38 +1035,50 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>0.15643000000000001</v>
+        <v>13</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0.16138</v>
       </c>
       <c r="F6">
-        <v>0.16766</v>
+        <v>0.16874</v>
       </c>
       <c r="G6">
-        <v>197</v>
+        <v>151</v>
       </c>
       <c r="J6">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0.15865000000000001</v>
+      </c>
+      <c r="F7">
+        <v>0.16622999999999999</v>
+      </c>
+      <c r="G7">
+        <v>149</v>
+      </c>
       <c r="J7">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8">
-        <v>0.16138</v>
+        <v>15</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0.15970999999999999</v>
       </c>
       <c r="F8">
-        <v>0.16874</v>
+        <v>0.16769000000000001</v>
       </c>
       <c r="G8">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="J8">
         <v>14</v>
@@ -1051,13 +1086,13 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9">
-        <v>0.15865000000000001</v>
+        <v>16</v>
+      </c>
+      <c r="E9" s="7">
+        <v>0.15970999999999999</v>
       </c>
       <c r="F9">
-        <v>0.16622999999999999</v>
+        <v>0.16621</v>
       </c>
       <c r="G9">
         <v>149</v>
@@ -1068,16 +1103,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10">
-        <v>0.15970999999999999</v>
+        <v>140</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0.16142999999999999</v>
       </c>
       <c r="F10">
-        <v>0.16769000000000001</v>
+        <v>0.17385</v>
       </c>
       <c r="G10">
-        <v>149</v>
+        <v>100</v>
       </c>
       <c r="J10">
         <v>14</v>
@@ -1085,16 +1120,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11">
-        <v>0.15970999999999999</v>
+        <v>141</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0.16051000000000001</v>
       </c>
       <c r="F11">
-        <v>0.16621</v>
+        <v>0.17383000000000001</v>
       </c>
       <c r="G11">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="J11">
         <v>14</v>
@@ -1102,16 +1137,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>140</v>
-      </c>
-      <c r="E12">
-        <v>0.16142999999999999</v>
+        <v>142</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.1585</v>
       </c>
       <c r="F12">
-        <v>0.17385</v>
+        <v>0.16952</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J12">
         <v>14</v>
@@ -1119,16 +1154,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>141</v>
-      </c>
-      <c r="E13">
-        <v>0.16051000000000001</v>
+        <v>143</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0.15845999999999999</v>
       </c>
       <c r="F13">
-        <v>0.17383000000000001</v>
+        <v>0.17163</v>
       </c>
       <c r="G13">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="J13">
         <v>14</v>
@@ -1136,16 +1171,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>142</v>
-      </c>
-      <c r="E14">
-        <v>0.1585</v>
+        <v>144</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.15742</v>
       </c>
       <c r="F14">
-        <v>0.16952</v>
+        <v>0.16646</v>
       </c>
       <c r="G14">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J14">
         <v>14</v>
@@ -1153,13 +1188,13 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15">
-        <v>0.15845999999999999</v>
+        <v>145</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0.156</v>
       </c>
       <c r="F15">
-        <v>0.17163</v>
+        <v>0.16458</v>
       </c>
       <c r="G15">
         <v>101</v>
@@ -1170,30 +1205,33 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>144</v>
-      </c>
-      <c r="E16">
-        <v>0.15742</v>
+        <v>146</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0.15608</v>
       </c>
       <c r="F16">
-        <v>0.16646</v>
+        <v>0.16475000000000001</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J16">
         <v>14</v>
+      </c>
+      <c r="K16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E17">
-        <v>0.156</v>
+        <v>147</v>
+      </c>
+      <c r="E17" s="7">
+        <v>0.15659999999999999</v>
       </c>
       <c r="F17">
-        <v>0.16458</v>
+        <v>0.16531999999999999</v>
       </c>
       <c r="G17">
         <v>101</v>
@@ -1201,76 +1239,73 @@
       <c r="J17">
         <v>14</v>
       </c>
+      <c r="K17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>146</v>
-      </c>
-      <c r="E18">
-        <v>0.15608</v>
+        <v>148</v>
+      </c>
+      <c r="E18" s="7">
+        <v>0.15604999999999999</v>
       </c>
       <c r="F18">
-        <v>0.16475000000000001</v>
+        <v>0.15941</v>
       </c>
       <c r="G18">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="J18">
-        <v>14</v>
-      </c>
-      <c r="K18" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>147</v>
-      </c>
-      <c r="E19">
-        <v>0.15659999999999999</v>
+        <v>149</v>
+      </c>
+      <c r="E19" s="7">
+        <v>0.15558</v>
       </c>
       <c r="F19">
-        <v>0.16531999999999999</v>
+        <v>0.15939999999999999</v>
       </c>
       <c r="G19">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="J19">
-        <v>14</v>
-      </c>
-      <c r="K19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20">
-        <v>0.15604999999999999</v>
+      <c r="C20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E20" s="7">
+        <v>0.15573999999999999</v>
       </c>
       <c r="F20">
-        <v>0.15941</v>
+        <v>0.15866</v>
       </c>
       <c r="G20">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J20">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21">
-        <v>0.15558</v>
+      <c r="C21" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E21" s="7">
+        <v>0.15884000000000001</v>
       </c>
       <c r="F21">
-        <v>0.15939999999999999</v>
+        <v>0.16170000000000001</v>
       </c>
       <c r="G21">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J21">
         <v>21</v>
@@ -1278,50 +1313,50 @@
     </row>
     <row r="22" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E22">
-        <v>0.15573999999999999</v>
+        <v>152</v>
+      </c>
+      <c r="E22" s="7">
+        <v>0.15834000000000001</v>
       </c>
       <c r="F22">
-        <v>0.15866</v>
+        <v>0.16292000000000001</v>
       </c>
       <c r="G22">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="J22">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23">
-        <v>0.15884000000000001</v>
+        <v>153</v>
+      </c>
+      <c r="E23" s="7">
+        <v>0.15851000000000001</v>
       </c>
       <c r="F23">
-        <v>0.16170000000000001</v>
+        <v>0.16272</v>
       </c>
       <c r="G23">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="J23">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E24">
-        <v>0.15834000000000001</v>
+        <v>154</v>
+      </c>
+      <c r="E24" s="7">
+        <v>0.15726999999999999</v>
       </c>
       <c r="F24">
-        <v>0.16292000000000001</v>
+        <v>0.16228000000000001</v>
       </c>
       <c r="G24">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J24">
         <v>14</v>
@@ -1329,67 +1364,67 @@
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E25">
-        <v>0.15851000000000001</v>
+        <v>155</v>
+      </c>
+      <c r="E25" s="7">
+        <v>0.15858</v>
       </c>
       <c r="F25">
-        <v>0.16272</v>
+        <v>0.16422</v>
       </c>
       <c r="G25">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="J25">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26">
-        <v>0.15726999999999999</v>
+        <v>30</v>
+      </c>
+      <c r="E26" s="7">
+        <v>0.15767</v>
       </c>
       <c r="F26">
-        <v>0.16228000000000001</v>
+        <v>0.15945999999999999</v>
       </c>
       <c r="G26">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="J26">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27">
-        <v>0.15858</v>
+        <v>31</v>
+      </c>
+      <c r="E27" s="7">
+        <v>0.15564</v>
       </c>
       <c r="F27">
-        <v>0.16422</v>
+        <v>0.15867000000000001</v>
       </c>
       <c r="G27">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="J27">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28">
-        <v>0.15767</v>
+        <v>32</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0.15520999999999999</v>
       </c>
       <c r="F28">
-        <v>0.15945999999999999</v>
+        <v>0.15821099999999999</v>
       </c>
       <c r="G28">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="J28">
         <v>7</v>
@@ -1397,13 +1432,13 @@
     </row>
     <row r="29" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E29">
-        <v>0.15564</v>
+        <v>33</v>
+      </c>
+      <c r="E29" s="7">
+        <v>0.15709000000000001</v>
       </c>
       <c r="F29">
-        <v>0.15867000000000001</v>
+        <v>0.1603</v>
       </c>
       <c r="G29">
         <v>150</v>
@@ -1414,50 +1449,50 @@
     </row>
     <row r="30" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30">
-        <v>0.15520999999999999</v>
+        <v>91</v>
+      </c>
+      <c r="E30" s="7">
+        <v>0.15787999999999999</v>
       </c>
       <c r="F30">
-        <v>0.15821099999999999</v>
+        <v>0.16320000000000001</v>
       </c>
       <c r="G30">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="J30">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E31">
-        <v>0.15709000000000001</v>
+        <v>92</v>
+      </c>
+      <c r="E31" s="7">
+        <v>0.15583</v>
       </c>
       <c r="F31">
-        <v>0.1603</v>
+        <v>0.16569</v>
       </c>
       <c r="G31">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="J31">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32">
-        <v>0.15787999999999999</v>
+        <v>93</v>
+      </c>
+      <c r="E32" s="7">
+        <v>0.16031000000000001</v>
       </c>
       <c r="F32">
-        <v>0.16320000000000001</v>
+        <v>0.16388</v>
       </c>
       <c r="G32">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J32">
         <v>14</v>
@@ -1465,13 +1500,13 @@
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33">
-        <v>0.15583</v>
+        <v>158</v>
+      </c>
+      <c r="E33" s="7">
+        <v>0.159</v>
       </c>
       <c r="F33">
-        <v>0.16569</v>
+        <v>0.16339999999999999</v>
       </c>
       <c r="G33">
         <v>100</v>
@@ -1482,16 +1517,16 @@
     </row>
     <row r="34" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34">
-        <v>0.16031000000000001</v>
+        <v>38</v>
+      </c>
+      <c r="E34" s="7">
+        <v>0.15572</v>
       </c>
       <c r="F34">
-        <v>0.16388</v>
+        <v>0.15801000000000001</v>
       </c>
       <c r="G34">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="J34">
         <v>14</v>
@@ -1499,16 +1534,16 @@
     </row>
     <row r="35" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="E35">
-        <v>0.159</v>
+        <v>39</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0.15558</v>
       </c>
       <c r="F35">
-        <v>0.16339999999999999</v>
+        <v>0.15790000000000001</v>
       </c>
       <c r="G35">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="J35">
         <v>14</v>
@@ -1516,16 +1551,16 @@
     </row>
     <row r="36" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E36">
-        <v>0.15572</v>
+        <v>40</v>
+      </c>
+      <c r="E36" s="7">
+        <v>0.15495</v>
       </c>
       <c r="F36">
-        <v>0.15801000000000001</v>
+        <v>0.13771</v>
       </c>
       <c r="G36">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J36">
         <v>14</v>
@@ -1533,13 +1568,13 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37">
-        <v>0.15558</v>
+        <v>156</v>
+      </c>
+      <c r="E37" s="7">
+        <v>0.15687999999999999</v>
       </c>
       <c r="F37">
-        <v>0.15790000000000001</v>
+        <v>0.15931999999999999</v>
       </c>
       <c r="G37">
         <v>75</v>
@@ -1550,50 +1585,56 @@
     </row>
     <row r="38" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E38">
-        <v>0.15495</v>
+        <v>35</v>
+      </c>
+      <c r="E38" s="7">
+        <v>0.15573999999999999</v>
       </c>
       <c r="F38">
-        <v>0.13771</v>
+        <v>0.1613</v>
       </c>
       <c r="G38">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="J38">
         <v>14</v>
+      </c>
+      <c r="K38" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E39">
-        <v>0.15687999999999999</v>
+        <v>36</v>
+      </c>
+      <c r="E39" s="7">
+        <v>0.15398999999999999</v>
       </c>
       <c r="F39">
-        <v>0.15931999999999999</v>
+        <v>0.15884000000000001</v>
       </c>
       <c r="G39">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="J39">
         <v>14</v>
+      </c>
+      <c r="K39" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E40">
-        <v>0.15573999999999999</v>
+        <v>37</v>
+      </c>
+      <c r="E40" s="7">
+        <v>0.15462000000000001</v>
       </c>
       <c r="F40">
-        <v>0.1613</v>
+        <v>0.16027</v>
       </c>
       <c r="G40">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J40">
         <v>14</v>
@@ -1604,16 +1645,16 @@
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41">
-        <v>0.15398999999999999</v>
+        <v>157</v>
+      </c>
+      <c r="E41" s="7">
+        <v>0.15362000000000001</v>
       </c>
       <c r="F41">
-        <v>0.15884000000000001</v>
+        <v>0.16027</v>
       </c>
       <c r="G41">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J41">
         <v>14</v>
@@ -1624,56 +1665,50 @@
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E42">
-        <v>0.15462000000000001</v>
+        <v>56</v>
+      </c>
+      <c r="E42" s="7">
+        <v>0.15822</v>
       </c>
       <c r="F42">
-        <v>0.16027</v>
+        <v>0.16250000000000001</v>
       </c>
       <c r="G42">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J42">
         <v>14</v>
-      </c>
-      <c r="K42" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="43" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="E43">
-        <v>0.15362000000000001</v>
+        <v>57</v>
+      </c>
+      <c r="E43" s="7">
+        <v>0.1575</v>
       </c>
       <c r="F43">
-        <v>0.16027</v>
+        <v>0.16222</v>
       </c>
       <c r="G43">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="J43">
         <v>14</v>
-      </c>
-      <c r="K43" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="44" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44">
-        <v>0.15822</v>
+        <v>58</v>
+      </c>
+      <c r="E44" s="7">
+        <v>0.15890000000000001</v>
       </c>
       <c r="F44">
-        <v>0.16250000000000001</v>
+        <v>0.16397999999999999</v>
       </c>
       <c r="G44">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="J44">
         <v>14</v>
@@ -1681,16 +1716,16 @@
     </row>
     <row r="45" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E45">
-        <v>0.1575</v>
+        <v>59</v>
+      </c>
+      <c r="E45" s="7">
+        <v>0.15909000000000001</v>
       </c>
       <c r="F45">
-        <v>0.16222</v>
+        <v>0.16452</v>
       </c>
       <c r="G45">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J45">
         <v>14</v>
@@ -1698,183 +1733,183 @@
     </row>
     <row r="46" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E46">
-        <v>0.15890000000000001</v>
+        <v>41</v>
+      </c>
+      <c r="E46" s="7">
+        <v>0.16075999999999999</v>
       </c>
       <c r="F46">
-        <v>0.16397999999999999</v>
+        <v>0.16372</v>
       </c>
       <c r="G46">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="J46">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E47">
-        <v>0.15909000000000001</v>
+        <v>41</v>
+      </c>
+      <c r="E47" s="7">
+        <v>0.15915000000000001</v>
       </c>
       <c r="F47">
-        <v>0.16452</v>
+        <v>0.16352</v>
       </c>
       <c r="G47">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J47">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E48">
-        <v>0.16075999999999999</v>
+        <v>42</v>
+      </c>
+      <c r="E48" s="7">
+        <v>0.15617</v>
       </c>
       <c r="F48">
-        <v>0.16372</v>
+        <v>0.161</v>
       </c>
       <c r="G48">
-        <v>46</v>
+        <v>86</v>
       </c>
       <c r="J48">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E49">
-        <v>0.15915000000000001</v>
+        <v>43</v>
+      </c>
+      <c r="E49" s="7">
+        <v>0.16111</v>
       </c>
       <c r="F49">
-        <v>0.16352</v>
+        <v>0.16603000000000001</v>
       </c>
       <c r="G49">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J49">
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E50">
-        <v>0.15617</v>
+        <v>44</v>
+      </c>
+      <c r="E50" s="7">
+        <v>0.16162000000000001</v>
       </c>
       <c r="F50">
-        <v>0.161</v>
+        <v>0.166603</v>
       </c>
       <c r="G50">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J50">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51">
-        <v>0.16111</v>
+        <v>45</v>
+      </c>
+      <c r="E51" s="7">
+        <v>0.156</v>
       </c>
       <c r="F51">
-        <v>0.16603000000000001</v>
+        <v>0.1666</v>
       </c>
       <c r="G51">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="J51">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E52">
-        <v>0.16162000000000001</v>
+        <v>46</v>
+      </c>
+      <c r="E52" s="7">
+        <v>0.15751999999999999</v>
       </c>
       <c r="F52">
-        <v>0.166603</v>
+        <v>0.16034999999999999</v>
       </c>
       <c r="G52">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="J52">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E53">
-        <v>0.156</v>
+        <v>47</v>
+      </c>
+      <c r="E53" s="7">
+        <v>0.15764</v>
       </c>
       <c r="F53">
-        <v>0.1666</v>
+        <v>0.16199</v>
       </c>
       <c r="G53">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="J53">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E54">
-        <v>0.15751999999999999</v>
+        <v>48</v>
+      </c>
+      <c r="E54" s="7">
+        <v>0.16083</v>
       </c>
       <c r="F54">
-        <v>0.16034999999999999</v>
+        <v>0.16739999999999999</v>
       </c>
       <c r="G54">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="J54">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E55">
-        <v>0.15764</v>
+        <v>48</v>
+      </c>
+      <c r="E55" s="7">
+        <v>0.15933</v>
       </c>
       <c r="F55">
-        <v>0.16199</v>
+        <v>0.10548</v>
       </c>
       <c r="G55">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J55">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E56">
-        <v>0.16083</v>
+        <v>49</v>
+      </c>
+      <c r="E56" s="7">
+        <v>0.15851000000000001</v>
       </c>
       <c r="F56">
-        <v>0.16739999999999999</v>
+        <v>0.1636</v>
       </c>
       <c r="G56">
         <v>50</v>
@@ -1883,358 +1918,400 @@
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E57">
-        <v>0.15933</v>
+        <v>50</v>
+      </c>
+      <c r="E57" s="7">
+        <v>0.15859999999999999</v>
       </c>
       <c r="F57">
-        <v>0.10548</v>
+        <v>0.16367000000000001</v>
       </c>
       <c r="G57">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="J57">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C58" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E58">
-        <v>0.15851000000000001</v>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>95</v>
+      </c>
+      <c r="E58" s="7">
+        <v>0.15584999999999999</v>
       </c>
       <c r="F58">
-        <v>0.1636</v>
+        <v>0.15847</v>
       </c>
       <c r="G58">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="J58">
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E59">
-        <v>0.15859999999999999</v>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="7">
+        <v>0.15423000000000001</v>
       </c>
       <c r="F59">
+        <v>0.15701999999999999</v>
+      </c>
+      <c r="G59">
+        <v>70</v>
+      </c>
+      <c r="J59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="7">
+        <v>0.15583</v>
+      </c>
+      <c r="F60">
+        <v>0.15817999999999999</v>
+      </c>
+      <c r="G60">
+        <v>69</v>
+      </c>
+      <c r="J60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.15587999999999999</v>
+      </c>
+      <c r="F61">
+        <v>0.15841</v>
+      </c>
+      <c r="G61">
+        <v>72</v>
+      </c>
+      <c r="J61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>99</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.16233</v>
+      </c>
+      <c r="F62">
+        <v>0.16699</v>
+      </c>
+      <c r="G62">
+        <v>68</v>
+      </c>
+      <c r="J62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.16169</v>
+      </c>
+      <c r="F63">
+        <v>0.16561999999999999</v>
+      </c>
+      <c r="G63">
+        <v>65</v>
+      </c>
+      <c r="J63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>159</v>
+      </c>
+      <c r="E64" s="7">
+        <v>0.15515000000000001</v>
+      </c>
+      <c r="F64">
+        <v>0.15945999999999999</v>
+      </c>
+      <c r="G64">
+        <v>64</v>
+      </c>
+      <c r="J64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>160</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0.15509000000000001</v>
+      </c>
+      <c r="F65">
+        <v>0.15905</v>
+      </c>
+      <c r="G65">
+        <v>66</v>
+      </c>
+      <c r="J65">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="7">
+        <v>0.15778</v>
+      </c>
+      <c r="F66">
+        <v>0.16339999999999999</v>
+      </c>
+      <c r="G66">
+        <v>76</v>
+      </c>
+      <c r="J66">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>101</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0.15565000000000001</v>
+      </c>
+      <c r="F67">
+        <v>0.16034999999999999</v>
+      </c>
+      <c r="G67">
+        <v>86</v>
+      </c>
+      <c r="J67">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>102</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0.15804000000000001</v>
+      </c>
+      <c r="F68">
+        <v>0.16608999999999999</v>
+      </c>
+      <c r="G68">
+        <v>75</v>
+      </c>
+      <c r="J68">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>103</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0.15684000000000001</v>
+      </c>
+      <c r="F69">
+        <v>0.16416</v>
+      </c>
+      <c r="G69">
+        <v>75</v>
+      </c>
+      <c r="J69">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>104</v>
+      </c>
+      <c r="E70" s="7">
+        <v>0.13755999999999999</v>
+      </c>
+      <c r="F70">
+        <v>0.17122999999999999</v>
+      </c>
+      <c r="G70">
+        <v>40</v>
+      </c>
+      <c r="J70">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>105</v>
+      </c>
+      <c r="E71" s="7">
+        <v>0.15445</v>
+      </c>
+      <c r="F71">
+        <v>0.16539999999999999</v>
+      </c>
+      <c r="G71">
+        <v>31</v>
+      </c>
+      <c r="J71">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="E72" s="7">
+        <v>0.16009000000000001</v>
+      </c>
+      <c r="F72">
+        <v>0.16852</v>
+      </c>
+      <c r="G72">
+        <v>38</v>
+      </c>
+      <c r="J72">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>107</v>
+      </c>
+      <c r="E73" s="7">
+        <v>0.16098999999999999</v>
+      </c>
+      <c r="F73">
+        <v>0.16628999999999999</v>
+      </c>
+      <c r="G73">
+        <v>29</v>
+      </c>
+      <c r="J73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>108</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0.15984999999999999</v>
+      </c>
+      <c r="F74">
+        <v>0.16464000000000001</v>
+      </c>
+      <c r="G74">
+        <v>70</v>
+      </c>
+      <c r="J74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>109</v>
+      </c>
+      <c r="E75" s="7">
+        <v>0.15867000000000001</v>
+      </c>
+      <c r="F75">
+        <v>0.16456999999999999</v>
+      </c>
+      <c r="G75">
+        <v>70</v>
+      </c>
+      <c r="J75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0.15931000000000001</v>
+      </c>
+      <c r="F76">
         <v>0.16367000000000001</v>
       </c>
-      <c r="G59">
-        <v>52</v>
-      </c>
-      <c r="J59">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F60">
-        <v>0.15726000000000001</v>
-      </c>
-      <c r="G60">
-        <v>50</v>
-      </c>
-      <c r="K60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F61">
-        <v>0.15479999999999999</v>
-      </c>
-      <c r="G61">
-        <v>55</v>
-      </c>
-      <c r="K61" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F62">
-        <v>0.15870000000000001</v>
-      </c>
-      <c r="G62">
-        <v>50</v>
-      </c>
-      <c r="K62" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="63" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F63">
-        <v>0.15689</v>
-      </c>
-      <c r="G63">
-        <v>50</v>
-      </c>
-      <c r="K63" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F64">
-        <v>0.15905</v>
-      </c>
-      <c r="G64">
-        <v>50</v>
-      </c>
-      <c r="K64" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F65">
-        <v>0.15745000000000001</v>
-      </c>
-      <c r="G65">
-        <v>50</v>
-      </c>
-      <c r="K65" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F66">
-        <v>0.15409</v>
-      </c>
-      <c r="G66">
-        <v>75</v>
-      </c>
-      <c r="K66" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="F67">
-        <v>0.15523999999999999</v>
-      </c>
-      <c r="G67">
-        <v>55</v>
-      </c>
-      <c r="K67" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C68" t="s">
-        <v>95</v>
-      </c>
-      <c r="E68">
-        <v>0.15584999999999999</v>
-      </c>
-      <c r="F68">
-        <v>0.15847</v>
-      </c>
-      <c r="G68">
-        <v>72</v>
-      </c>
-      <c r="J68">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C69" t="s">
-        <v>96</v>
-      </c>
-      <c r="E69">
-        <v>0.15423000000000001</v>
-      </c>
-      <c r="F69">
-        <v>0.15701999999999999</v>
-      </c>
-      <c r="G69">
-        <v>70</v>
-      </c>
-      <c r="J69">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="70" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C70" t="s">
-        <v>97</v>
-      </c>
-      <c r="E70">
-        <v>0.15583</v>
-      </c>
-      <c r="F70">
-        <v>0.15817999999999999</v>
-      </c>
-      <c r="G70">
-        <v>69</v>
-      </c>
-      <c r="J70">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C71" t="s">
-        <v>98</v>
-      </c>
-      <c r="E71">
-        <v>0.15587999999999999</v>
-      </c>
-      <c r="F71">
-        <v>0.15841</v>
-      </c>
-      <c r="G71">
-        <v>72</v>
-      </c>
-      <c r="J71">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C72" t="s">
-        <v>99</v>
-      </c>
-      <c r="E72">
-        <v>0.16233</v>
-      </c>
-      <c r="G72">
-        <v>68</v>
-      </c>
-      <c r="J72">
-        <v>14</v>
-      </c>
-      <c r="K72" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="73" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C73" t="s">
-        <v>99</v>
-      </c>
-      <c r="E73">
-        <v>0.16169</v>
-      </c>
-      <c r="F73">
-        <v>0.16561999999999999</v>
-      </c>
-      <c r="G73">
-        <v>65</v>
-      </c>
-      <c r="J73">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C74" t="s">
-        <v>99</v>
-      </c>
-      <c r="E74">
-        <v>0.15515000000000001</v>
-      </c>
-      <c r="F74">
-        <v>0.15945999999999999</v>
-      </c>
-      <c r="G74">
-        <v>64</v>
-      </c>
-      <c r="J74">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C75" t="s">
-        <v>99</v>
-      </c>
-      <c r="E75">
-        <v>0.15509000000000001</v>
-      </c>
-      <c r="F75">
-        <v>0.15905</v>
-      </c>
-      <c r="G75">
-        <v>66</v>
-      </c>
-      <c r="J75">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C76" t="s">
-        <v>100</v>
-      </c>
-      <c r="E76">
-        <v>0.15778</v>
-      </c>
-      <c r="F76">
-        <v>0.16339999999999999</v>
-      </c>
       <c r="G76">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J76">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>101</v>
-      </c>
-      <c r="E77">
-        <v>0.15565000000000001</v>
+        <v>111</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0.15812999999999999</v>
       </c>
       <c r="F77">
-        <v>0.16034999999999999</v>
+        <v>0.16428999999999999</v>
       </c>
       <c r="G77">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="J77">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C78" t="s">
-        <v>102</v>
-      </c>
-      <c r="E78">
-        <v>0.15804000000000001</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C78" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0.15898999999999999</v>
       </c>
       <c r="F78">
-        <v>0.16608999999999999</v>
+        <v>0.16284999999999999</v>
       </c>
       <c r="G78">
-        <v>75</v>
+        <v>40</v>
       </c>
       <c r="J78">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="79" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C79" t="s">
-        <v>103</v>
-      </c>
-      <c r="E79">
-        <v>0.15684000000000001</v>
-      </c>
-      <c r="F79">
-        <v>0.16416</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C79" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E79" s="7">
+        <v>0.16089000000000001</v>
       </c>
       <c r="G79">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="J79">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C80" t="s">
-        <v>104</v>
-      </c>
-      <c r="E80">
-        <v>0.13755999999999999</v>
-      </c>
-      <c r="F80">
-        <v>0.17122999999999999</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C80" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E80" s="7">
+        <v>0.16186</v>
       </c>
       <c r="G80">
         <v>40</v>
@@ -2244,119 +2321,119 @@
       </c>
     </row>
     <row r="81" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C81" t="s">
-        <v>105</v>
-      </c>
-      <c r="E81">
-        <v>0.15445</v>
+      <c r="C81" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E81" s="7">
+        <v>0.16017000000000001</v>
       </c>
       <c r="F81">
-        <v>0.16539999999999999</v>
+        <v>0.16567999999999999</v>
       </c>
       <c r="G81">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="J81">
         <v>14</v>
       </c>
     </row>
     <row r="82" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C82" t="s">
-        <v>106</v>
-      </c>
-      <c r="E82">
-        <v>0.16009000000000001</v>
+      <c r="C82" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E82" s="7">
+        <v>0.15820000000000001</v>
       </c>
       <c r="F82">
-        <v>0.16852</v>
+        <v>0.16291</v>
       </c>
       <c r="G82">
-        <v>38</v>
+        <v>101</v>
       </c>
       <c r="J82">
         <v>14</v>
       </c>
     </row>
     <row r="83" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C83" t="s">
-        <v>107</v>
-      </c>
-      <c r="E83">
-        <v>0.16098999999999999</v>
+      <c r="C83" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E83" s="7">
+        <v>0.15794</v>
       </c>
       <c r="F83">
-        <v>0.16628999999999999</v>
+        <v>0.16320000000000001</v>
       </c>
       <c r="G83">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="J83">
         <v>14</v>
       </c>
     </row>
     <row r="84" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C84" t="s">
-        <v>108</v>
-      </c>
-      <c r="E84">
-        <v>0.15984999999999999</v>
+      <c r="C84" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E84" s="7">
+        <v>0.15837999999999999</v>
       </c>
       <c r="F84">
-        <v>0.16464000000000001</v>
+        <v>0.16186</v>
       </c>
       <c r="G84">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="J84">
         <v>14</v>
       </c>
     </row>
     <row r="85" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C85" t="s">
-        <v>109</v>
-      </c>
-      <c r="E85">
-        <v>0.15867000000000001</v>
+      <c r="C85" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E85" s="7">
+        <v>0.15840000000000001</v>
       </c>
       <c r="F85">
-        <v>0.16456999999999999</v>
+        <v>0.16184000000000001</v>
       </c>
       <c r="G85">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="J85">
         <v>14</v>
       </c>
     </row>
     <row r="86" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C86" t="s">
-        <v>110</v>
-      </c>
-      <c r="E86">
-        <v>0.15931000000000001</v>
+      <c r="C86" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E86" s="7">
+        <v>0.15612999999999999</v>
       </c>
       <c r="F86">
-        <v>0.16367000000000001</v>
+        <v>0.16184000000000001</v>
       </c>
       <c r="G86">
-        <v>77</v>
+        <v>50</v>
       </c>
       <c r="J86">
         <v>14</v>
       </c>
     </row>
     <row r="87" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C87" t="s">
-        <v>111</v>
-      </c>
-      <c r="E87">
-        <v>0.15812999999999999</v>
+      <c r="C87" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E87" s="7">
+        <v>0.13650000000000001</v>
       </c>
       <c r="F87">
-        <v>0.16428999999999999</v>
+        <v>0.16245999999999999</v>
       </c>
       <c r="G87">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="J87">
         <v>14</v>
@@ -2364,16 +2441,16 @@
     </row>
     <row r="88" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E88">
-        <v>0.15898999999999999</v>
+        <v>122</v>
+      </c>
+      <c r="E88" s="7">
+        <v>0.15742</v>
       </c>
       <c r="F88">
-        <v>0.16284999999999999</v>
+        <v>0.16263</v>
       </c>
       <c r="G88">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="J88">
         <v>14</v>
@@ -2381,13 +2458,16 @@
     </row>
     <row r="89" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E89">
-        <v>0.16089000000000001</v>
+        <v>123</v>
+      </c>
+      <c r="E89" s="7">
+        <v>0.15698000000000001</v>
+      </c>
+      <c r="F89">
+        <v>0.16225999999999999</v>
       </c>
       <c r="G89">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="J89">
         <v>14</v>
@@ -2395,428 +2475,273 @@
     </row>
     <row r="90" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E90">
-        <v>0.16186</v>
+        <v>124</v>
+      </c>
+      <c r="E90" s="7">
+        <v>0.15665999999999999</v>
+      </c>
+      <c r="F90">
+        <v>0.15956999999999999</v>
       </c>
       <c r="G90">
-        <v>40</v>
+        <v>129</v>
       </c>
       <c r="J90">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="91" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E91">
-        <v>0.16017000000000001</v>
+        <v>125</v>
+      </c>
+      <c r="E91" s="7">
+        <v>0.15712999999999999</v>
       </c>
       <c r="F91">
-        <v>0.16567999999999999</v>
+        <v>0.1593</v>
       </c>
       <c r="G91">
-        <v>40</v>
+        <v>151</v>
       </c>
       <c r="J91">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="92" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="E92">
-        <v>0.15820000000000001</v>
+        <v>126</v>
+      </c>
+      <c r="E92" s="7">
+        <v>0.1573</v>
       </c>
       <c r="F92">
-        <v>0.16291</v>
+        <v>0.15947</v>
+      </c>
+      <c r="G92">
+        <v>87</v>
       </c>
       <c r="J92">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E93">
-        <v>0.15794</v>
+        <v>127</v>
+      </c>
+      <c r="E93" s="7">
+        <v>0.15776999999999999</v>
       </c>
       <c r="F93">
-        <v>0.16320000000000001</v>
+        <v>0.15970999999999999</v>
+      </c>
+      <c r="G93">
+        <v>135</v>
       </c>
       <c r="J93">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E94">
-        <v>0.15837999999999999</v>
+        <v>128</v>
+      </c>
+      <c r="E94" s="7">
+        <v>0.158</v>
       </c>
       <c r="F94">
-        <v>0.16186</v>
+        <v>0.16849</v>
+      </c>
+      <c r="G94">
+        <v>60</v>
       </c>
       <c r="J94">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E95">
-        <v>0.15840000000000001</v>
+        <v>129</v>
+      </c>
+      <c r="E95" s="7">
+        <v>0.15770000000000001</v>
       </c>
       <c r="F95">
-        <v>0.16184000000000001</v>
+        <v>0.16799</v>
+      </c>
+      <c r="G95">
+        <v>60</v>
       </c>
       <c r="J95">
-        <v>14</v>
+        <v>42</v>
       </c>
     </row>
     <row r="96" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E96" s="7">
+        <v>0.15664</v>
+      </c>
+      <c r="F96">
+        <v>0.16767000000000001</v>
+      </c>
+      <c r="G96">
+        <v>60</v>
+      </c>
+      <c r="J96">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C97" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E97" s="7">
+        <v>0.15640000000000001</v>
+      </c>
+      <c r="F97">
+        <v>0.1663</v>
+      </c>
+      <c r="G97">
+        <v>60</v>
+      </c>
+      <c r="J97">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C98" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E98" s="7">
+        <v>0.15523000000000001</v>
+      </c>
+      <c r="F98">
+        <v>0.16098000000000001</v>
+      </c>
+      <c r="G98">
+        <v>97</v>
+      </c>
+      <c r="J98">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C99" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E99" s="7">
+        <v>0.15554000000000001</v>
+      </c>
+      <c r="F99">
+        <v>0.16142999999999999</v>
+      </c>
+      <c r="G99">
+        <v>100</v>
+      </c>
+      <c r="J99">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C100" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E100" s="7">
+        <v>0.15518000000000001</v>
+      </c>
+      <c r="F100">
+        <v>0.16142999999999999</v>
+      </c>
+      <c r="G100">
+        <v>100</v>
+      </c>
+      <c r="J100">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C101" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E101" s="7">
+        <v>0.15368000000000001</v>
+      </c>
+      <c r="F101">
+        <v>0.15926999999999999</v>
+      </c>
+      <c r="G101">
+        <v>100</v>
+      </c>
+      <c r="J101">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C102" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E102" s="7">
+        <v>0.15484000000000001</v>
+      </c>
+      <c r="F102">
+        <v>0.16116</v>
+      </c>
+      <c r="G102">
+        <v>100</v>
+      </c>
+      <c r="J102">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C103" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E103" s="7">
+        <v>0.15522</v>
+      </c>
+      <c r="F103">
+        <v>0.16186</v>
+      </c>
+      <c r="G103">
         <v>120</v>
       </c>
-      <c r="E96">
-        <v>0.15612999999999999</v>
-      </c>
-      <c r="F96">
-        <v>0.16184000000000001</v>
-      </c>
-      <c r="G96">
-        <v>50</v>
-      </c>
-      <c r="J96">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C97" s="2" t="s">
+      <c r="J103">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C104" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E104" s="7">
+        <v>0.15653</v>
+      </c>
+      <c r="F104">
+        <v>0.16450000000000001</v>
+      </c>
+      <c r="G104">
+        <v>151</v>
+      </c>
+      <c r="J104">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C105" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E105" s="7">
+        <v>0.15406</v>
+      </c>
+      <c r="F105">
+        <v>0.16012000000000001</v>
+      </c>
+      <c r="G105">
         <v>121</v>
       </c>
-      <c r="E97">
-        <v>0.13650000000000001</v>
-      </c>
-      <c r="F97">
-        <v>0.16245999999999999</v>
-      </c>
-      <c r="G97">
-        <v>51</v>
-      </c>
-      <c r="J97">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C98" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="E98">
-        <v>0.15742</v>
-      </c>
-      <c r="F98">
-        <v>0.16263</v>
-      </c>
-      <c r="G98">
-        <v>52</v>
-      </c>
-      <c r="J98">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C99" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E99">
-        <v>0.15698000000000001</v>
-      </c>
-      <c r="F99">
-        <v>0.16225999999999999</v>
-      </c>
-      <c r="G99">
-        <v>52</v>
-      </c>
-      <c r="J99">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C100" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E100">
-        <v>0.15665999999999999</v>
-      </c>
-      <c r="F100">
-        <v>0.15956999999999999</v>
-      </c>
-      <c r="G100">
-        <v>129</v>
-      </c>
-      <c r="J100">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="101" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C101" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E101">
-        <v>0.15712999999999999</v>
-      </c>
-      <c r="F101">
-        <v>0.1593</v>
-      </c>
-      <c r="G101">
-        <v>151</v>
-      </c>
-      <c r="J101">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="102" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C102" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E102">
-        <v>0.1573</v>
-      </c>
-      <c r="F102">
-        <v>0.15947</v>
-      </c>
-      <c r="G102">
-        <v>87</v>
-      </c>
-      <c r="J102">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C103" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E103">
-        <v>0.15776999999999999</v>
-      </c>
-      <c r="F103">
-        <v>0.15970999999999999</v>
-      </c>
-      <c r="G103">
-        <v>135</v>
-      </c>
-      <c r="J103">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C104" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F104">
-        <v>0.16849</v>
-      </c>
-      <c r="G104">
-        <v>60</v>
-      </c>
-      <c r="J104">
-        <v>42</v>
-      </c>
-      <c r="K104" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="105" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C105" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F105">
-        <v>0.16799</v>
-      </c>
-      <c r="G105">
-        <v>60</v>
-      </c>
       <c r="J105">
-        <v>42</v>
-      </c>
-      <c r="K105" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="106" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C106" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F106">
-        <v>0.16767000000000001</v>
-      </c>
-      <c r="G106">
-        <v>60</v>
-      </c>
-      <c r="J106">
-        <v>42</v>
-      </c>
-      <c r="K106" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="107" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C107" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F107">
-        <v>0.1663</v>
-      </c>
-      <c r="G107">
-        <v>60</v>
-      </c>
-      <c r="J107">
-        <v>42</v>
-      </c>
-      <c r="K107" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="108" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C108" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="E108">
-        <v>0.15523000000000001</v>
-      </c>
-      <c r="F108">
-        <v>0.16098000000000001</v>
-      </c>
-      <c r="G108">
-        <v>97</v>
-      </c>
-      <c r="J108">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="109" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C109" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E109">
-        <v>0.15554000000000001</v>
-      </c>
-      <c r="F109">
-        <v>0.16142999999999999</v>
-      </c>
-      <c r="G109">
-        <v>100</v>
-      </c>
-      <c r="J109">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="110" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C110" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E110">
-        <v>0.15518000000000001</v>
-      </c>
-      <c r="F110">
-        <v>0.16142999999999999</v>
-      </c>
-      <c r="G110">
-        <v>100</v>
-      </c>
-      <c r="J110">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="111" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C111" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E111">
-        <v>0.15368000000000001</v>
-      </c>
-      <c r="F111">
-        <v>0.15926999999999999</v>
-      </c>
-      <c r="G111">
-        <v>100</v>
-      </c>
-      <c r="J111">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="112" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="C112" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="E112">
-        <v>0.15484000000000001</v>
-      </c>
-      <c r="F112">
-        <v>0.16116</v>
-      </c>
-      <c r="G112">
-        <v>100</v>
-      </c>
-      <c r="J112">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="113" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C113" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="E113">
-        <v>0.15522</v>
-      </c>
-      <c r="F113">
-        <v>0.16186</v>
-      </c>
-      <c r="G113">
-        <v>120</v>
-      </c>
-      <c r="J113">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="114" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C114" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="E114">
-        <v>0.15653</v>
-      </c>
-      <c r="F114">
-        <v>0.16450000000000001</v>
-      </c>
-      <c r="G114">
-        <v>151</v>
-      </c>
-      <c r="J114">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="115" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C115" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="E115">
-        <v>0.15406</v>
-      </c>
-      <c r="F115">
-        <v>0.16012000000000001</v>
-      </c>
-      <c r="G115">
-        <v>121</v>
-      </c>
-      <c r="J115">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
So many errors to fix!
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAABB8DD-1993-CA47-82F0-C04EA5EF5867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50640C2F-AAFF-1A4C-BF2D-488BB06C7A1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
@@ -505,9 +505,6 @@
     <t>F_Sed_8m_R2_F7_25Jun18</t>
   </si>
   <si>
-    <t>F_Sed_4m_R2_F8_25Jun18</t>
-  </si>
-  <si>
     <t>F_Sed_4m_R2_F4_16Jul18</t>
   </si>
   <si>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t>B_Sed_4m_R2_F3_07Sep18</t>
+  </si>
+  <si>
+    <t>F_Sed_8m_R2_F8_25Jun18</t>
   </si>
 </sst>
 </file>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1465,7 @@
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="E25" s="7">
         <v>0.15858</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="33" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E33" s="7">
         <v>0.159</v>
@@ -1717,7 +1717,7 @@
     </row>
     <row r="37" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E37" s="7">
         <v>0.15687999999999999</v>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="41" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E41" s="7">
         <v>0.15362000000000001</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="47" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E47" s="7">
         <v>0.15915000000000001</v>
@@ -2107,7 +2107,7 @@
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E55" s="7">
         <v>0.15933</v>
@@ -2275,7 +2275,7 @@
     </row>
     <row r="63" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E63" s="7">
         <v>0.16169</v>
@@ -2296,7 +2296,7 @@
     </row>
     <row r="64" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E64" s="7">
         <v>0.15515000000000001</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="65" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E65" s="7">
         <v>0.15509000000000001</v>
@@ -4069,7 +4069,7 @@
         <v>0.15931999999999999</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -4170,7 +4170,7 @@
         <v>0.16027</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Fixing errors for EDI
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66CC089-4ECC-5543-893D-1269D8BDBBD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E186CF-5CC9-D746-862E-92C87726148E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1481,7 +1481,7 @@
         <v>5.6400000000000061E-3</v>
       </c>
       <c r="J25">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed raw sed trap files to match most current naming format.
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cecewood/Documents/GitHub/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E186CF-5CC9-D746-862E-92C87726148E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA95595-E60C-784B-9B75-79D4ACB2DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="166">
   <si>
     <t>Collection Day</t>
   </si>
@@ -271,30 +271,6 @@
     <t>Initials</t>
   </si>
   <si>
-    <t>Date_Filtered</t>
-  </si>
-  <si>
-    <t>Sample_ID</t>
-  </si>
-  <si>
-    <t>Pan_Mass_g</t>
-  </si>
-  <si>
-    <t>Filter_mass_pre_filtering_g</t>
-  </si>
-  <si>
-    <t>Filter_mass_post_filtering_g</t>
-  </si>
-  <si>
-    <t>Volume_filtered_mL</t>
-  </si>
-  <si>
-    <t>Volume_discarded_mL</t>
-  </si>
-  <si>
-    <t>Mass_of_sediment_g</t>
-  </si>
-  <si>
     <t>Duration_days</t>
   </si>
   <si>
@@ -530,6 +506,36 @@
   </si>
   <si>
     <t>F_Sed_8m_R2_F8_25Jun18</t>
+  </si>
+  <si>
+    <t>PanMass_g</t>
+  </si>
+  <si>
+    <t>FilterMassPre_g</t>
+  </si>
+  <si>
+    <t>FilterMassPost_g</t>
+  </si>
+  <si>
+    <t>FilterVol_mL</t>
+  </si>
+  <si>
+    <t>VolDiscarded_mL</t>
+  </si>
+  <si>
+    <t>SedMass_g</t>
+  </si>
+  <si>
+    <t>VolDiscarded_L</t>
+  </si>
+  <si>
+    <t>FilterVol_L</t>
+  </si>
+  <si>
+    <t>DateFiltered</t>
+  </si>
+  <si>
+    <t>FilterID</t>
   </si>
 </sst>
 </file>
@@ -624,9 +630,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -664,7 +670,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -770,7 +776,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -912,7 +918,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -920,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC1477B9-ED04-AF45-983E-E50DF958859A}">
-  <dimension ref="A1:K105"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -933,50 +939,56 @@
     <col min="4" max="4" width="10.83203125" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" style="7" customWidth="1"/>
     <col min="6" max="6" width="25.1640625" customWidth="1"/>
-    <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="18.1640625" customWidth="1"/>
+    <col min="9" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="M1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
         <v>78</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C2" t="s">
-        <v>86</v>
       </c>
       <c r="E2" s="7">
         <v>0.15815000000000001</v>
@@ -987,15 +999,19 @@
       <c r="G2">
         <v>200</v>
       </c>
-      <c r="I2" s="7">
+      <c r="H2">
+        <f>G2/1000</f>
+        <v>0.2</v>
+      </c>
+      <c r="K2" s="7">
         <f>F2-E2</f>
         <v>1.121999999999998E-2</v>
       </c>
-      <c r="J2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -1008,15 +1024,19 @@
       <c r="G3">
         <v>202</v>
       </c>
-      <c r="I3" s="7">
-        <f t="shared" ref="I3:I66" si="0">F3-E3</f>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="0">G3/1000</f>
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K66" si="1">F3-E3</f>
         <v>1.2479999999999991E-2</v>
       </c>
-      <c r="J3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>11</v>
       </c>
@@ -1029,15 +1049,19 @@
       <c r="G4">
         <v>197</v>
       </c>
-      <c r="I4" s="7">
+      <c r="H4">
         <f t="shared" si="0"/>
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="1"/>
         <v>1.2190000000000006E-2</v>
       </c>
-      <c r="J4">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>12</v>
       </c>
@@ -1050,15 +1074,19 @@
       <c r="G5">
         <v>197</v>
       </c>
-      <c r="I5" s="7">
+      <c r="H5">
         <f t="shared" si="0"/>
+        <v>0.19700000000000001</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="1"/>
         <v>1.122999999999999E-2</v>
       </c>
-      <c r="J5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>13</v>
       </c>
@@ -1071,15 +1099,19 @@
       <c r="G6">
         <v>151</v>
       </c>
-      <c r="I6" s="7">
+      <c r="H6">
         <f t="shared" si="0"/>
+        <v>0.151</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="1"/>
         <v>7.3600000000000054E-3</v>
       </c>
-      <c r="J6">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>14</v>
       </c>
@@ -1092,15 +1124,19 @@
       <c r="G7">
         <v>149</v>
       </c>
-      <c r="I7" s="7">
+      <c r="H7">
         <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K7" s="7">
+        <f t="shared" si="1"/>
         <v>7.5799999999999756E-3</v>
       </c>
-      <c r="J7">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>15</v>
       </c>
@@ -1113,15 +1149,19 @@
       <c r="G8">
         <v>149</v>
       </c>
-      <c r="I8" s="7">
+      <c r="H8">
         <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K8" s="7">
+        <f t="shared" si="1"/>
         <v>7.9800000000000149E-3</v>
       </c>
-      <c r="J8">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>16</v>
       </c>
@@ -1134,17 +1174,21 @@
       <c r="G9">
         <v>149</v>
       </c>
-      <c r="I9" s="7">
+      <c r="H9">
         <f t="shared" si="0"/>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="K9" s="7">
+        <f t="shared" si="1"/>
         <v>6.5000000000000058E-3</v>
       </c>
-      <c r="J9">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="E10" s="7">
         <v>0.16142999999999999</v>
@@ -1155,17 +1199,21 @@
       <c r="G10">
         <v>100</v>
       </c>
-      <c r="I10" s="7">
+      <c r="H10">
         <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" si="1"/>
         <v>1.2420000000000014E-2</v>
       </c>
-      <c r="J10">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E11" s="7">
         <v>0.16051000000000001</v>
@@ -1176,17 +1224,21 @@
       <c r="G11">
         <v>99</v>
       </c>
-      <c r="I11" s="7">
+      <c r="H11">
         <f t="shared" si="0"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="1"/>
         <v>1.3319999999999999E-2</v>
       </c>
-      <c r="J11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E12" s="7">
         <v>0.1585</v>
@@ -1197,17 +1249,21 @@
       <c r="G12">
         <v>101</v>
       </c>
-      <c r="I12" s="7">
+      <c r="H12">
         <f t="shared" si="0"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K12" s="7">
+        <f t="shared" si="1"/>
         <v>1.1020000000000002E-2</v>
       </c>
-      <c r="J12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E13" s="7">
         <v>0.15845999999999999</v>
@@ -1218,17 +1274,21 @@
       <c r="G13">
         <v>101</v>
       </c>
-      <c r="I13" s="7">
+      <c r="H13">
         <f t="shared" si="0"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="1"/>
         <v>1.3170000000000015E-2</v>
       </c>
-      <c r="J13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E14" s="7">
         <v>0.15742</v>
@@ -1239,17 +1299,21 @@
       <c r="G14">
         <v>100</v>
       </c>
-      <c r="I14" s="7">
+      <c r="H14">
         <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="1"/>
         <v>9.0399999999999925E-3</v>
       </c>
-      <c r="J14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E15" s="7">
         <v>0.156</v>
@@ -1260,17 +1324,21 @@
       <c r="G15">
         <v>101</v>
       </c>
-      <c r="I15" s="7">
+      <c r="H15">
         <f t="shared" si="0"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K15" s="7">
+        <f t="shared" si="1"/>
         <v>8.5800000000000043E-3</v>
       </c>
-      <c r="J15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E16" s="7">
         <v>0.15608</v>
@@ -1281,20 +1349,24 @@
       <c r="G16">
         <v>99</v>
       </c>
-      <c r="I16" s="7">
+      <c r="H16">
         <f t="shared" si="0"/>
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K16" s="7">
+        <f t="shared" si="1"/>
         <v>8.670000000000011E-3</v>
       </c>
-      <c r="J16">
-        <v>14</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="L16">
+        <v>14</v>
+      </c>
+      <c r="M16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="E17" s="7">
         <v>0.15659999999999999</v>
@@ -1305,20 +1377,24 @@
       <c r="G17">
         <v>101</v>
       </c>
-      <c r="I17" s="7">
+      <c r="H17">
         <f t="shared" si="0"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K17" s="7">
+        <f t="shared" si="1"/>
         <v>8.7200000000000055E-3</v>
       </c>
-      <c r="J17">
-        <v>14</v>
-      </c>
-      <c r="K17" t="s">
+      <c r="L17">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E18" s="7">
         <v>0.15604999999999999</v>
@@ -1329,17 +1405,21 @@
       <c r="G18">
         <v>85</v>
       </c>
-      <c r="I18" s="7">
+      <c r="H18">
         <f t="shared" si="0"/>
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K18" s="7">
+        <f t="shared" si="1"/>
         <v>3.3600000000000019E-3</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E19" s="7">
         <v>0.15558</v>
@@ -1350,17 +1430,21 @@
       <c r="G19">
         <v>87</v>
       </c>
-      <c r="I19" s="7">
+      <c r="H19">
         <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="1"/>
         <v>3.8199999999999901E-3</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C20" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="E20" s="7">
         <v>0.15573999999999999</v>
@@ -1371,17 +1455,21 @@
       <c r="G20">
         <v>84</v>
       </c>
-      <c r="I20" s="7">
+      <c r="H20">
         <f t="shared" si="0"/>
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="1"/>
         <v>2.9200000000000059E-3</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C21" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E21" s="7">
         <v>0.15884000000000001</v>
@@ -1392,17 +1480,21 @@
       <c r="G21">
         <v>86</v>
       </c>
-      <c r="I21" s="7">
+      <c r="H21">
         <f t="shared" si="0"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="1"/>
         <v>2.8600000000000014E-3</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C22" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="E22" s="7">
         <v>0.15834000000000001</v>
@@ -1413,17 +1505,21 @@
       <c r="G22">
         <v>80</v>
       </c>
-      <c r="I22" s="7">
+      <c r="H22">
         <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="K22" s="7">
+        <f t="shared" si="1"/>
         <v>4.5800000000000007E-3</v>
       </c>
-      <c r="J22">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="E23" s="7">
         <v>0.15851000000000001</v>
@@ -1434,17 +1530,21 @@
       <c r="G23">
         <v>79</v>
       </c>
-      <c r="I23" s="7">
+      <c r="H23">
         <f t="shared" si="0"/>
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K23" s="7">
+        <f t="shared" si="1"/>
         <v>4.2099999999999915E-3</v>
       </c>
-      <c r="J23">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E24" s="7">
         <v>0.15726999999999999</v>
@@ -1455,17 +1555,21 @@
       <c r="G24">
         <v>79</v>
       </c>
-      <c r="I24" s="7">
+      <c r="H24">
         <f t="shared" si="0"/>
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="K24" s="7">
+        <f t="shared" si="1"/>
         <v>5.0100000000000144E-3</v>
       </c>
-      <c r="J24">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C25" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E25" s="7">
         <v>0.15858</v>
@@ -1476,15 +1580,19 @@
       <c r="G25">
         <v>80</v>
       </c>
-      <c r="I25" s="7">
+      <c r="H25">
         <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="K25" s="7">
+        <f t="shared" si="1"/>
         <v>5.6400000000000061E-3</v>
       </c>
-      <c r="J25">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1497,15 +1605,19 @@
       <c r="G26">
         <v>150</v>
       </c>
-      <c r="I26" s="7">
+      <c r="H26">
         <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="K26" s="7">
+        <f t="shared" si="1"/>
         <v>1.789999999999986E-3</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1518,15 +1630,19 @@
       <c r="G27">
         <v>150</v>
       </c>
-      <c r="I27" s="7">
+      <c r="H27">
         <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="K27" s="7">
+        <f t="shared" si="1"/>
         <v>3.0300000000000049E-3</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1539,15 +1655,19 @@
       <c r="G28">
         <v>153</v>
       </c>
-      <c r="I28" s="7">
+      <c r="H28">
         <f t="shared" si="0"/>
+        <v>0.153</v>
+      </c>
+      <c r="K28" s="7">
+        <f t="shared" si="1"/>
         <v>3.0010000000000037E-3</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1560,17 +1680,21 @@
       <c r="G29">
         <v>150</v>
       </c>
-      <c r="I29" s="7">
+      <c r="H29">
         <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="1"/>
         <v>3.2099999999999906E-3</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="E30" s="7">
         <v>0.15787999999999999</v>
@@ -1581,17 +1705,21 @@
       <c r="G30">
         <v>100</v>
       </c>
-      <c r="I30" s="7">
+      <c r="H30">
         <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K30" s="7">
+        <f t="shared" si="1"/>
         <v>5.3200000000000192E-3</v>
       </c>
-      <c r="J30">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C31" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E31" s="7">
         <v>0.15583</v>
@@ -1602,17 +1730,21 @@
       <c r="G31">
         <v>100</v>
       </c>
-      <c r="I31" s="7">
+      <c r="H31">
         <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K31" s="7">
+        <f t="shared" si="1"/>
         <v>9.8600000000000076E-3</v>
       </c>
-      <c r="J31">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L31">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="E32" s="7">
         <v>0.16031000000000001</v>
@@ -1623,17 +1755,21 @@
       <c r="G32">
         <v>98</v>
       </c>
-      <c r="I32" s="7">
+      <c r="H32">
         <f t="shared" si="0"/>
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="K32" s="7">
+        <f t="shared" si="1"/>
         <v>3.5699999999999898E-3</v>
       </c>
-      <c r="J32">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C33" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="E33" s="7">
         <v>0.159</v>
@@ -1644,15 +1780,19 @@
       <c r="G33">
         <v>100</v>
       </c>
-      <c r="I33" s="7">
+      <c r="H33">
         <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="K33" s="7">
+        <f t="shared" si="1"/>
         <v>4.3999999999999873E-3</v>
       </c>
-      <c r="J33">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1665,15 +1805,19 @@
       <c r="G34">
         <v>76</v>
       </c>
-      <c r="I34" s="7">
+      <c r="H34">
         <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K34" s="7">
+        <f t="shared" si="1"/>
         <v>2.2900000000000142E-3</v>
       </c>
-      <c r="J34">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1686,15 +1830,19 @@
       <c r="G35">
         <v>75</v>
       </c>
-      <c r="I35" s="7">
+      <c r="H35">
         <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K35" s="7">
+        <f t="shared" si="1"/>
         <v>2.3200000000000165E-3</v>
       </c>
-      <c r="J35">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1707,17 +1855,21 @@
       <c r="G36">
         <v>77</v>
       </c>
-      <c r="I36" s="7">
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="K36" s="7">
         <f>F36-E36</f>
         <v>2.7599999999999847E-3</v>
       </c>
-      <c r="J36">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C37" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E37" s="7">
         <v>0.15687999999999999</v>
@@ -1728,15 +1880,19 @@
       <c r="G37">
         <v>75</v>
       </c>
-      <c r="I37" s="7">
+      <c r="H37">
         <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" si="1"/>
         <v>2.4399999999999977E-3</v>
       </c>
-      <c r="J37">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C38" s="2" t="s">
         <v>35</v>
       </c>
@@ -1749,18 +1905,22 @@
       <c r="G38">
         <v>50</v>
       </c>
-      <c r="I38" s="7">
+      <c r="H38">
         <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="1"/>
         <v>5.5600000000000094E-3</v>
       </c>
-      <c r="J38">
-        <v>14</v>
-      </c>
-      <c r="K38" t="s">
+      <c r="L38">
+        <v>14</v>
+      </c>
+      <c r="M38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C39" s="2" t="s">
         <v>36</v>
       </c>
@@ -1773,18 +1933,22 @@
       <c r="G39">
         <v>51</v>
       </c>
-      <c r="I39" s="7">
+      <c r="H39">
         <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="1"/>
         <v>4.850000000000021E-3</v>
       </c>
-      <c r="J39">
-        <v>14</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="L39">
+        <v>14</v>
+      </c>
+      <c r="M39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C40" s="2" t="s">
         <v>37</v>
       </c>
@@ -1797,20 +1961,24 @@
       <c r="G40">
         <v>53</v>
       </c>
-      <c r="I40" s="7">
+      <c r="H40">
         <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K40" s="7">
+        <f t="shared" si="1"/>
         <v>5.6499999999999884E-3</v>
       </c>
-      <c r="J40">
-        <v>14</v>
-      </c>
-      <c r="K40" t="s">
+      <c r="L40">
+        <v>14</v>
+      </c>
+      <c r="M40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C41" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E41" s="7">
         <v>0.15362000000000001</v>
@@ -1821,18 +1989,22 @@
       <c r="G41">
         <v>52</v>
       </c>
-      <c r="I41" s="7">
+      <c r="H41">
         <f t="shared" si="0"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K41" s="7">
+        <f t="shared" si="1"/>
         <v>6.6499999999999893E-3</v>
       </c>
-      <c r="J41">
-        <v>14</v>
-      </c>
-      <c r="K41" t="s">
+      <c r="L41">
+        <v>14</v>
+      </c>
+      <c r="M41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C42" s="2" t="s">
         <v>56</v>
       </c>
@@ -1845,15 +2017,19 @@
       <c r="G42">
         <v>55</v>
       </c>
-      <c r="I42" s="7">
+      <c r="H42">
         <f t="shared" si="0"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="K42" s="7">
+        <f t="shared" si="1"/>
         <v>4.280000000000006E-3</v>
       </c>
-      <c r="J42">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C43" s="2" t="s">
         <v>57</v>
       </c>
@@ -1866,15 +2042,19 @@
       <c r="G43">
         <v>56</v>
       </c>
-      <c r="I43" s="7">
+      <c r="H43">
         <f t="shared" si="0"/>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="K43" s="7">
+        <f t="shared" si="1"/>
         <v>4.720000000000002E-3</v>
       </c>
-      <c r="J43">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L43">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C44" s="2" t="s">
         <v>58</v>
       </c>
@@ -1887,15 +2067,19 @@
       <c r="G44">
         <v>66</v>
       </c>
-      <c r="I44" s="7">
+      <c r="H44">
         <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K44" s="7">
+        <f t="shared" si="1"/>
         <v>5.0799999999999734E-3</v>
       </c>
-      <c r="J44">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C45" s="2" t="s">
         <v>59</v>
       </c>
@@ -1908,15 +2092,19 @@
       <c r="G45">
         <v>59</v>
       </c>
-      <c r="I45" s="7">
+      <c r="H45">
         <f t="shared" si="0"/>
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K45" s="7">
+        <f t="shared" si="1"/>
         <v>5.4299999999999904E-3</v>
       </c>
-      <c r="J45">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="L45">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C46" s="2" t="s">
         <v>41</v>
       </c>
@@ -1929,17 +2117,21 @@
       <c r="G46">
         <v>46</v>
       </c>
-      <c r="I46" s="7">
+      <c r="H46">
         <f t="shared" si="0"/>
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="K46" s="7">
+        <f t="shared" si="1"/>
         <v>2.9600000000000182E-3</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C47" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="E47" s="7">
         <v>0.15915000000000001</v>
@@ -1950,15 +2142,19 @@
       <c r="G47">
         <v>53</v>
       </c>
-      <c r="I47" s="7">
+      <c r="H47">
         <f t="shared" si="0"/>
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="K47" s="7">
+        <f t="shared" si="1"/>
         <v>4.369999999999985E-3</v>
       </c>
-      <c r="J47">
+      <c r="L47">
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C48" s="2" t="s">
         <v>42</v>
       </c>
@@ -1971,15 +2167,19 @@
       <c r="G48">
         <v>86</v>
       </c>
-      <c r="I48" s="7">
+      <c r="H48">
         <f t="shared" si="0"/>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K48" s="7">
+        <f t="shared" si="1"/>
         <v>4.830000000000001E-3</v>
       </c>
-      <c r="J48">
+      <c r="L48">
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C49" s="2" t="s">
         <v>43</v>
       </c>
@@ -1992,15 +2192,19 @@
       <c r="G49">
         <v>51</v>
       </c>
-      <c r="I49" s="7">
+      <c r="H49">
         <f t="shared" si="0"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K49" s="7">
+        <f t="shared" si="1"/>
         <v>4.9200000000000077E-3</v>
       </c>
-      <c r="J49">
+      <c r="L49">
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C50" s="2" t="s">
         <v>44</v>
       </c>
@@ -2013,15 +2217,19 @@
       <c r="G50">
         <v>87</v>
       </c>
-      <c r="I50" s="7">
+      <c r="H50">
         <f t="shared" si="0"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K50" s="7">
+        <f t="shared" si="1"/>
         <v>4.9829999999999874E-3</v>
       </c>
-      <c r="J50">
+      <c r="L50">
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C51" s="2" t="s">
         <v>45</v>
       </c>
@@ -2034,15 +2242,19 @@
       <c r="G51">
         <v>68</v>
       </c>
-      <c r="I51" s="7">
+      <c r="H51">
         <f t="shared" si="0"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K51" s="7">
+        <f t="shared" si="1"/>
         <v>1.0599999999999998E-2</v>
       </c>
-      <c r="J51">
+      <c r="L51">
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C52" s="2" t="s">
         <v>46</v>
       </c>
@@ -2055,15 +2267,19 @@
       <c r="G52">
         <v>76</v>
       </c>
-      <c r="I52" s="7">
+      <c r="H52">
         <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K52" s="7">
+        <f t="shared" si="1"/>
         <v>2.8299999999999992E-3</v>
       </c>
-      <c r="J52">
+      <c r="L52">
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C53" s="2" t="s">
         <v>47</v>
       </c>
@@ -2076,15 +2292,19 @@
       <c r="G53">
         <v>80</v>
       </c>
-      <c r="I53" s="7">
+      <c r="H53">
         <f t="shared" si="0"/>
+        <v>0.08</v>
+      </c>
+      <c r="K53" s="7">
+        <f t="shared" si="1"/>
         <v>4.3499999999999928E-3</v>
       </c>
-      <c r="J53">
+      <c r="L53">
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C54" s="2" t="s">
         <v>48</v>
       </c>
@@ -2097,17 +2317,21 @@
       <c r="G54">
         <v>50</v>
       </c>
-      <c r="I54" s="7">
+      <c r="H54">
         <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="K54" s="7">
+        <f t="shared" si="1"/>
         <v>6.5699999999999925E-3</v>
       </c>
-      <c r="J54">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L54">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C55" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="E55" s="7">
         <v>0.15933</v>
@@ -2118,15 +2342,19 @@
       <c r="G55">
         <v>50</v>
       </c>
-      <c r="I55" s="7">
+      <c r="H55">
         <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="K55" s="7">
+        <f t="shared" si="1"/>
         <v>6.1499999999999888E-3</v>
       </c>
-      <c r="J55">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L55">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C56" s="2" t="s">
         <v>49</v>
       </c>
@@ -2139,15 +2367,19 @@
       <c r="G56">
         <v>50</v>
       </c>
-      <c r="I56" s="7">
+      <c r="H56">
         <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
+      <c r="K56" s="7">
+        <f t="shared" si="1"/>
         <v>5.0899999999999834E-3</v>
       </c>
-      <c r="J56">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C57" s="2" t="s">
         <v>50</v>
       </c>
@@ -2160,17 +2392,21 @@
       <c r="G57">
         <v>52</v>
       </c>
-      <c r="I57" s="7">
+      <c r="H57">
         <f t="shared" si="0"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K57" s="7">
+        <f t="shared" si="1"/>
         <v>5.0700000000000189E-3</v>
       </c>
-      <c r="J57">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L57">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="E58" s="7">
         <v>0.15584999999999999</v>
@@ -2181,17 +2417,21 @@
       <c r="G58">
         <v>72</v>
       </c>
-      <c r="I58" s="7">
+      <c r="H58">
         <f t="shared" si="0"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K58" s="7">
+        <f t="shared" si="1"/>
         <v>2.6200000000000112E-3</v>
       </c>
-      <c r="J58">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L58">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E59" s="7">
         <v>0.15423000000000001</v>
@@ -2202,17 +2442,21 @@
       <c r="G59">
         <v>70</v>
       </c>
-      <c r="I59" s="7">
+      <c r="H59">
         <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K59" s="7">
+        <f t="shared" si="1"/>
         <v>2.7899999999999869E-3</v>
       </c>
-      <c r="J59">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E60" s="7">
         <v>0.15583</v>
@@ -2223,17 +2467,21 @@
       <c r="G60">
         <v>69</v>
       </c>
-      <c r="I60" s="7">
+      <c r="H60">
         <f t="shared" si="0"/>
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="K60" s="7">
+        <f t="shared" si="1"/>
         <v>2.349999999999991E-3</v>
       </c>
-      <c r="J60">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E61" s="7">
         <v>0.15587999999999999</v>
@@ -2244,17 +2492,21 @@
       <c r="G61">
         <v>72</v>
       </c>
-      <c r="I61" s="7">
+      <c r="H61">
         <f t="shared" si="0"/>
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K61" s="7">
+        <f t="shared" si="1"/>
         <v>2.5300000000000045E-3</v>
       </c>
-      <c r="J61">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L61">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E62" s="7">
         <v>0.16233</v>
@@ -2265,17 +2517,21 @@
       <c r="G62">
         <v>68</v>
       </c>
-      <c r="I62" s="7">
+      <c r="H62">
         <f t="shared" si="0"/>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="K62" s="7">
+        <f t="shared" si="1"/>
         <v>4.6599999999999975E-3</v>
       </c>
-      <c r="J62">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="E63" s="7">
         <v>0.16169</v>
@@ -2286,17 +2542,21 @@
       <c r="G63">
         <v>65</v>
       </c>
-      <c r="I63" s="7">
+      <c r="H63">
         <f t="shared" si="0"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="K63" s="7">
+        <f t="shared" si="1"/>
         <v>3.9299999999999891E-3</v>
       </c>
-      <c r="J63">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="E64" s="7">
         <v>0.15515000000000001</v>
@@ -2307,17 +2567,21 @@
       <c r="G64">
         <v>64</v>
       </c>
-      <c r="I64" s="7">
+      <c r="H64">
         <f t="shared" si="0"/>
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="K64" s="7">
+        <f t="shared" si="1"/>
         <v>4.3099999999999805E-3</v>
       </c>
-      <c r="J64">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L64">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="E65" s="7">
         <v>0.15509000000000001</v>
@@ -2328,17 +2592,21 @@
       <c r="G65">
         <v>66</v>
       </c>
-      <c r="I65" s="7">
+      <c r="H65">
         <f t="shared" si="0"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="K65" s="7">
+        <f t="shared" si="1"/>
         <v>3.9599999999999913E-3</v>
       </c>
-      <c r="J65">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L65">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="E66" s="7">
         <v>0.15778</v>
@@ -2349,17 +2617,21 @@
       <c r="G66">
         <v>76</v>
       </c>
-      <c r="I66" s="7">
+      <c r="H66">
         <f t="shared" si="0"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="K66" s="7">
+        <f t="shared" si="1"/>
         <v>5.6199999999999861E-3</v>
       </c>
-      <c r="J66">
+      <c r="L66">
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E67" s="7">
         <v>0.15565000000000001</v>
@@ -2370,17 +2642,21 @@
       <c r="G67">
         <v>86</v>
       </c>
-      <c r="I67" s="7">
-        <f t="shared" ref="I67:I105" si="1">F67-E67</f>
+      <c r="H67">
+        <f t="shared" ref="H67:H105" si="2">G67/1000</f>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K67" s="7">
+        <f t="shared" ref="K67:K105" si="3">F67-E67</f>
         <v>4.699999999999982E-3</v>
       </c>
-      <c r="J67">
+      <c r="L67">
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="E68" s="7">
         <v>0.15804000000000001</v>
@@ -2391,17 +2667,21 @@
       <c r="G68">
         <v>75</v>
       </c>
-      <c r="I68" s="7">
-        <f t="shared" si="1"/>
+      <c r="H68">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K68" s="7">
+        <f t="shared" si="3"/>
         <v>8.0499999999999738E-3</v>
       </c>
-      <c r="J68">
+      <c r="L68">
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E69" s="7">
         <v>0.15684000000000001</v>
@@ -2412,17 +2692,21 @@
       <c r="G69">
         <v>75</v>
       </c>
-      <c r="I69" s="7">
-        <f t="shared" si="1"/>
+      <c r="H69">
+        <f t="shared" si="2"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="K69" s="7">
+        <f t="shared" si="3"/>
         <v>7.3199999999999932E-3</v>
       </c>
-      <c r="J69">
+      <c r="L69">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="E70" s="7">
         <v>0.13755999999999999</v>
@@ -2433,17 +2717,21 @@
       <c r="G70">
         <v>40</v>
       </c>
-      <c r="I70" s="7">
-        <f t="shared" si="1"/>
+      <c r="H70">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="K70" s="7">
+        <f t="shared" si="3"/>
         <v>3.3670000000000005E-2</v>
       </c>
-      <c r="J70">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L70">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="E71" s="7">
         <v>0.15445</v>
@@ -2454,17 +2742,21 @@
       <c r="G71">
         <v>31</v>
       </c>
-      <c r="I71" s="7">
-        <f t="shared" si="1"/>
+      <c r="H71">
+        <f t="shared" si="2"/>
+        <v>3.1E-2</v>
+      </c>
+      <c r="K71" s="7">
+        <f t="shared" si="3"/>
         <v>1.0949999999999988E-2</v>
       </c>
-      <c r="J71">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L71">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E72" s="7">
         <v>0.16009000000000001</v>
@@ -2475,17 +2767,21 @@
       <c r="G72">
         <v>38</v>
       </c>
-      <c r="I72" s="7">
-        <f t="shared" si="1"/>
+      <c r="H72">
+        <f t="shared" si="2"/>
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="K72" s="7">
+        <f t="shared" si="3"/>
         <v>8.4299999999999931E-3</v>
       </c>
-      <c r="J72">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L72">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E73" s="7">
         <v>0.16098999999999999</v>
@@ -2496,17 +2792,21 @@
       <c r="G73">
         <v>29</v>
       </c>
-      <c r="I73" s="7">
-        <f t="shared" si="1"/>
+      <c r="H73">
+        <f t="shared" si="2"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="K73" s="7">
+        <f t="shared" si="3"/>
         <v>5.2999999999999992E-3</v>
       </c>
-      <c r="J73">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L73">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E74" s="7">
         <v>0.15984999999999999</v>
@@ -2517,17 +2817,21 @@
       <c r="G74">
         <v>70</v>
       </c>
-      <c r="I74" s="7">
-        <f t="shared" si="1"/>
+      <c r="H74">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K74" s="7">
+        <f t="shared" si="3"/>
         <v>4.7900000000000165E-3</v>
       </c>
-      <c r="J74">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E75" s="7">
         <v>0.15867000000000001</v>
@@ -2538,17 +2842,21 @@
       <c r="G75">
         <v>70</v>
       </c>
-      <c r="I75" s="7">
-        <f t="shared" si="1"/>
+      <c r="H75">
+        <f t="shared" si="2"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K75" s="7">
+        <f t="shared" si="3"/>
         <v>5.8999999999999886E-3</v>
       </c>
-      <c r="J75">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L75">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E76" s="7">
         <v>0.15931000000000001</v>
@@ -2559,17 +2867,21 @@
       <c r="G76">
         <v>77</v>
       </c>
-      <c r="I76" s="7">
-        <f t="shared" si="1"/>
+      <c r="H76">
+        <f t="shared" si="2"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="K76" s="7">
+        <f t="shared" si="3"/>
         <v>4.3600000000000028E-3</v>
       </c>
-      <c r="J76">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L76">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="E77" s="7">
         <v>0.15812999999999999</v>
@@ -2580,17 +2892,21 @@
       <c r="G77">
         <v>78</v>
       </c>
-      <c r="I77" s="7">
-        <f t="shared" si="1"/>
+      <c r="H77">
+        <f t="shared" si="2"/>
+        <v>7.8E-2</v>
+      </c>
+      <c r="K77" s="7">
+        <f t="shared" si="3"/>
         <v>6.1599999999999988E-3</v>
       </c>
-      <c r="J77">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L77">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C78" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="E78" s="7">
         <v>0.15898999999999999</v>
@@ -2601,17 +2917,21 @@
       <c r="G78">
         <v>40</v>
       </c>
-      <c r="I78" s="7">
-        <f t="shared" si="1"/>
+      <c r="H78">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="K78" s="7">
+        <f t="shared" si="3"/>
         <v>3.8600000000000023E-3</v>
       </c>
-      <c r="J78">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L78">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C79" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E79" s="7">
         <v>0.16089000000000001</v>
@@ -2619,14 +2939,18 @@
       <c r="G79">
         <v>42</v>
       </c>
-      <c r="I79" s="7"/>
-      <c r="J79">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H79">
+        <f t="shared" si="2"/>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="K79" s="7"/>
+      <c r="L79">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="80" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C80" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E80" s="7">
         <v>0.16186</v>
@@ -2634,14 +2958,18 @@
       <c r="G80">
         <v>40</v>
       </c>
-      <c r="I80" s="7"/>
-      <c r="J80">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="H80">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="K80" s="7"/>
+      <c r="L80">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C81" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="E81" s="7">
         <v>0.16017000000000001</v>
@@ -2652,17 +2980,21 @@
       <c r="G81">
         <v>40</v>
       </c>
-      <c r="I81" s="7">
-        <f t="shared" si="1"/>
+      <c r="H81">
+        <f t="shared" si="2"/>
+        <v>0.04</v>
+      </c>
+      <c r="K81" s="7">
+        <f t="shared" si="3"/>
         <v>5.5099999999999871E-3</v>
       </c>
-      <c r="J81">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L81">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="82" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C82" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="E82" s="7">
         <v>0.15820000000000001</v>
@@ -2673,17 +3005,21 @@
       <c r="G82">
         <v>101</v>
       </c>
-      <c r="I82" s="7">
-        <f t="shared" si="1"/>
+      <c r="H82">
+        <f t="shared" si="2"/>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K82" s="7">
+        <f t="shared" si="3"/>
         <v>4.709999999999992E-3</v>
       </c>
-      <c r="J82">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L82">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C83" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E83" s="7">
         <v>0.15794</v>
@@ -2694,17 +3030,21 @@
       <c r="G83">
         <v>100</v>
       </c>
-      <c r="I83" s="7">
-        <f t="shared" si="1"/>
+      <c r="H83">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K83" s="7">
+        <f t="shared" si="3"/>
         <v>5.2600000000000147E-3</v>
       </c>
-      <c r="J83">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L83">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C84" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E84" s="7">
         <v>0.15837999999999999</v>
@@ -2715,17 +3055,21 @@
       <c r="G84">
         <v>200</v>
       </c>
-      <c r="I84" s="7">
-        <f t="shared" si="1"/>
+      <c r="H84">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+      <c r="K84" s="7">
+        <f t="shared" si="3"/>
         <v>3.4800000000000109E-3</v>
       </c>
-      <c r="J84">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L84">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="85" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C85" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E85" s="7">
         <v>0.15840000000000001</v>
@@ -2736,17 +3080,21 @@
       <c r="G85">
         <v>100</v>
       </c>
-      <c r="I85" s="7">
-        <f t="shared" si="1"/>
+      <c r="H85">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K85" s="7">
+        <f t="shared" si="3"/>
         <v>3.4399999999999986E-3</v>
       </c>
-      <c r="J85">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L85">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="86" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C86" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="E86" s="7">
         <v>0.15612999999999999</v>
@@ -2757,17 +3105,21 @@
       <c r="G86">
         <v>50</v>
       </c>
-      <c r="I86" s="7">
-        <f t="shared" si="1"/>
+      <c r="H86">
+        <f t="shared" si="2"/>
+        <v>0.05</v>
+      </c>
+      <c r="K86" s="7">
+        <f t="shared" si="3"/>
         <v>5.7100000000000206E-3</v>
       </c>
-      <c r="J86">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L86">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C87" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="E87" s="7">
         <v>0.13650000000000001</v>
@@ -2778,17 +3130,21 @@
       <c r="G87">
         <v>51</v>
       </c>
-      <c r="I87" s="7">
-        <f t="shared" si="1"/>
+      <c r="H87">
+        <f t="shared" si="2"/>
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="K87" s="7">
+        <f t="shared" si="3"/>
         <v>2.5959999999999983E-2</v>
       </c>
-      <c r="J87">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L87">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C88" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E88" s="7">
         <v>0.15742</v>
@@ -2799,17 +3155,21 @@
       <c r="G88">
         <v>52</v>
       </c>
-      <c r="I88" s="7">
-        <f t="shared" si="1"/>
+      <c r="H88">
+        <f t="shared" si="2"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K88" s="7">
+        <f t="shared" si="3"/>
         <v>5.2099999999999924E-3</v>
       </c>
-      <c r="J88">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L88">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="89" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C89" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E89" s="7">
         <v>0.15698000000000001</v>
@@ -2820,17 +3180,21 @@
       <c r="G89">
         <v>52</v>
       </c>
-      <c r="I89" s="7">
-        <f t="shared" si="1"/>
+      <c r="H89">
+        <f t="shared" si="2"/>
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="K89" s="7">
+        <f t="shared" si="3"/>
         <v>5.2799999999999792E-3</v>
       </c>
-      <c r="J89">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="L89">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C90" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E90" s="7">
         <v>0.15665999999999999</v>
@@ -2841,17 +3205,21 @@
       <c r="G90">
         <v>129</v>
       </c>
-      <c r="I90" s="7">
-        <f t="shared" si="1"/>
+      <c r="H90">
+        <f t="shared" si="2"/>
+        <v>0.129</v>
+      </c>
+      <c r="K90" s="7">
+        <f t="shared" si="3"/>
         <v>2.9099999999999959E-3</v>
       </c>
-      <c r="J90">
+      <c r="L90">
         <v>35</v>
       </c>
     </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C91" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E91" s="7">
         <v>0.15712999999999999</v>
@@ -2862,17 +3230,21 @@
       <c r="G91">
         <v>151</v>
       </c>
-      <c r="I91" s="7">
-        <f t="shared" si="1"/>
+      <c r="H91">
+        <f t="shared" si="2"/>
+        <v>0.151</v>
+      </c>
+      <c r="K91" s="7">
+        <f t="shared" si="3"/>
         <v>2.1700000000000053E-3</v>
       </c>
-      <c r="J91">
+      <c r="L91">
         <v>35</v>
       </c>
     </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C92" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E92" s="7">
         <v>0.1573</v>
@@ -2883,17 +3255,21 @@
       <c r="G92">
         <v>87</v>
       </c>
-      <c r="I92" s="7">
-        <f t="shared" si="1"/>
+      <c r="H92">
+        <f t="shared" si="2"/>
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K92" s="7">
+        <f t="shared" si="3"/>
         <v>2.1700000000000053E-3</v>
       </c>
-      <c r="J92">
+      <c r="L92">
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C93" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E93" s="7">
         <v>0.15776999999999999</v>
@@ -2904,17 +3280,21 @@
       <c r="G93">
         <v>135</v>
       </c>
-      <c r="I93" s="7">
-        <f t="shared" si="1"/>
+      <c r="H93">
+        <f t="shared" si="2"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="K93" s="7">
+        <f t="shared" si="3"/>
         <v>1.9399999999999973E-3</v>
       </c>
-      <c r="J93">
+      <c r="L93">
         <v>35</v>
       </c>
     </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C94" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E94" s="7">
         <v>0.158</v>
@@ -2925,17 +3305,21 @@
       <c r="G94">
         <v>60</v>
       </c>
-      <c r="I94" s="7">
-        <f t="shared" si="1"/>
+      <c r="H94">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="K94" s="7">
+        <f t="shared" si="3"/>
         <v>1.0489999999999999E-2</v>
       </c>
-      <c r="J94">
+      <c r="L94">
         <v>42</v>
       </c>
     </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C95" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E95" s="7">
         <v>0.15770000000000001</v>
@@ -2946,17 +3330,21 @@
       <c r="G95">
         <v>60</v>
       </c>
-      <c r="I95" s="7">
-        <f t="shared" si="1"/>
+      <c r="H95">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="K95" s="7">
+        <f t="shared" si="3"/>
         <v>1.0289999999999994E-2</v>
       </c>
-      <c r="J95">
+      <c r="L95">
         <v>42</v>
       </c>
     </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C96" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="E96" s="7">
         <v>0.15664</v>
@@ -2967,17 +3355,21 @@
       <c r="G96">
         <v>60</v>
       </c>
-      <c r="I96" s="7">
-        <f t="shared" si="1"/>
+      <c r="H96">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="K96" s="7">
+        <f t="shared" si="3"/>
         <v>1.1030000000000012E-2</v>
       </c>
-      <c r="J96">
+      <c r="L96">
         <v>42</v>
       </c>
     </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C97" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="E97" s="7">
         <v>0.15640000000000001</v>
@@ -2988,17 +3380,21 @@
       <c r="G97">
         <v>60</v>
       </c>
-      <c r="I97" s="7">
-        <f t="shared" si="1"/>
+      <c r="H97">
+        <f t="shared" si="2"/>
+        <v>0.06</v>
+      </c>
+      <c r="K97" s="7">
+        <f t="shared" si="3"/>
         <v>9.8999999999999921E-3</v>
       </c>
-      <c r="J97">
+      <c r="L97">
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C98" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E98" s="7">
         <v>0.15523000000000001</v>
@@ -3009,17 +3405,21 @@
       <c r="G98">
         <v>97</v>
       </c>
-      <c r="I98" s="7">
-        <f t="shared" si="1"/>
+      <c r="H98">
+        <f t="shared" si="2"/>
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="K98" s="7">
+        <f t="shared" si="3"/>
         <v>5.7500000000000051E-3</v>
       </c>
-      <c r="J98">
+      <c r="L98">
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C99" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E99" s="7">
         <v>0.15554000000000001</v>
@@ -3030,17 +3430,21 @@
       <c r="G99">
         <v>100</v>
       </c>
-      <c r="I99" s="7">
-        <f t="shared" si="1"/>
+      <c r="H99">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K99" s="7">
+        <f t="shared" si="3"/>
         <v>5.8899999999999786E-3</v>
       </c>
-      <c r="J99">
+      <c r="L99">
         <v>7</v>
       </c>
     </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C100" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E100" s="7">
         <v>0.15518000000000001</v>
@@ -3051,17 +3455,21 @@
       <c r="G100">
         <v>100</v>
       </c>
-      <c r="I100" s="7">
-        <f t="shared" si="1"/>
+      <c r="H100">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K100" s="7">
+        <f t="shared" si="3"/>
         <v>6.2499999999999778E-3</v>
       </c>
-      <c r="J100">
+      <c r="L100">
         <v>7</v>
       </c>
     </row>
-    <row r="101" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C101" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E101" s="7">
         <v>0.15368000000000001</v>
@@ -3072,17 +3480,21 @@
       <c r="G101">
         <v>100</v>
       </c>
-      <c r="I101" s="7">
-        <f t="shared" si="1"/>
+      <c r="H101">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K101" s="7">
+        <f t="shared" si="3"/>
         <v>5.5899999999999839E-3</v>
       </c>
-      <c r="J101">
+      <c r="L101">
         <v>7</v>
       </c>
     </row>
-    <row r="102" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C102" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E102" s="7">
         <v>0.15484000000000001</v>
@@ -3093,17 +3505,21 @@
       <c r="G102">
         <v>100</v>
       </c>
-      <c r="I102" s="7">
-        <f t="shared" si="1"/>
+      <c r="H102">
+        <f t="shared" si="2"/>
+        <v>0.1</v>
+      </c>
+      <c r="K102" s="7">
+        <f t="shared" si="3"/>
         <v>6.3199999999999923E-3</v>
       </c>
-      <c r="J102">
+      <c r="L102">
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C103" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E103" s="7">
         <v>0.15522</v>
@@ -3114,17 +3530,21 @@
       <c r="G103">
         <v>120</v>
       </c>
-      <c r="I103" s="7">
-        <f t="shared" si="1"/>
+      <c r="H103">
+        <f t="shared" si="2"/>
+        <v>0.12</v>
+      </c>
+      <c r="K103" s="7">
+        <f t="shared" si="3"/>
         <v>6.640000000000007E-3</v>
       </c>
-      <c r="J103">
+      <c r="L103">
         <v>21</v>
       </c>
     </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C104" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E104" s="7">
         <v>0.15653</v>
@@ -3135,17 +3555,21 @@
       <c r="G104">
         <v>151</v>
       </c>
-      <c r="I104" s="7">
-        <f t="shared" si="1"/>
+      <c r="H104">
+        <f t="shared" si="2"/>
+        <v>0.151</v>
+      </c>
+      <c r="K104" s="7">
+        <f t="shared" si="3"/>
         <v>7.9700000000000049E-3</v>
       </c>
-      <c r="J104">
+      <c r="L104">
         <v>21</v>
       </c>
     </row>
-    <row r="105" spans="3:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C105" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="E105" s="7">
         <v>0.15406</v>
@@ -3156,11 +3580,15 @@
       <c r="G105">
         <v>121</v>
       </c>
-      <c r="I105" s="7">
-        <f t="shared" si="1"/>
+      <c r="H105">
+        <f t="shared" si="2"/>
+        <v>0.121</v>
+      </c>
+      <c r="K105" s="7">
+        <f t="shared" si="3"/>
         <v>6.0600000000000098E-3</v>
       </c>
-      <c r="J105">
+      <c r="L105">
         <v>21</v>
       </c>
     </row>
@@ -3236,7 +3664,7 @@
         <v>0.16936999999999999</v>
       </c>
       <c r="H2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3442,7 +3870,7 @@
         <v>0.17385</v>
       </c>
       <c r="H12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -3465,7 +3893,7 @@
         <v>0.17383000000000001</v>
       </c>
       <c r="H13" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -3488,7 +3916,7 @@
         <v>0.16952</v>
       </c>
       <c r="H14" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -3511,7 +3939,7 @@
         <v>0.17163</v>
       </c>
       <c r="H15" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -3908,7 +4336,7 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
@@ -3931,7 +4359,7 @@
         <v>0.16569</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
@@ -3954,7 +4382,7 @@
         <v>0.16388</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
@@ -3977,7 +4405,7 @@
         <v>0.16339999999999999</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -4069,7 +4497,7 @@
         <v>0.15931999999999999</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
@@ -4170,7 +4598,7 @@
         <v>0.16027</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I43" t="s">
         <v>34</v>
@@ -4724,7 +5152,7 @@
         <v>0.15847</v>
       </c>
       <c r="H68" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -4747,7 +5175,7 @@
         <v>0.15701999999999999</v>
       </c>
       <c r="H69" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -4770,7 +5198,7 @@
         <v>0.15817999999999999</v>
       </c>
       <c r="H70" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -4793,7 +5221,7 @@
         <v>0.15841</v>
       </c>
       <c r="H71" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -4813,7 +5241,7 @@
         <v>0.16233</v>
       </c>
       <c r="H72" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>53</v>
@@ -4839,7 +5267,7 @@
         <v>0.16561999999999999</v>
       </c>
       <c r="H73" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -4862,7 +5290,7 @@
         <v>0.15945999999999999</v>
       </c>
       <c r="H74" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -4885,7 +5313,7 @@
         <v>0.15905</v>
       </c>
       <c r="H75" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -4908,7 +5336,7 @@
         <v>0.16339999999999999</v>
       </c>
       <c r="H76" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -4931,7 +5359,7 @@
         <v>0.16034999999999999</v>
       </c>
       <c r="H77" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -4954,7 +5382,7 @@
         <v>0.16608999999999999</v>
       </c>
       <c r="H78" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -4977,7 +5405,7 @@
         <v>0.16416</v>
       </c>
       <c r="H79" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -5000,7 +5428,7 @@
         <v>0.17122999999999999</v>
       </c>
       <c r="H80" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -5023,7 +5451,7 @@
         <v>0.16539999999999999</v>
       </c>
       <c r="H81" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -5046,7 +5474,7 @@
         <v>0.16852</v>
       </c>
       <c r="H82" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -5069,7 +5497,7 @@
         <v>0.16628999999999999</v>
       </c>
       <c r="H83" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -5092,7 +5520,7 @@
         <v>0.16464000000000001</v>
       </c>
       <c r="H84" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -5115,7 +5543,7 @@
         <v>0.16456999999999999</v>
       </c>
       <c r="H85" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -5138,7 +5566,7 @@
         <v>0.16367000000000001</v>
       </c>
       <c r="H86" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -5161,7 +5589,7 @@
         <v>0.16428999999999999</v>
       </c>
       <c r="H87" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -5184,7 +5612,7 @@
         <v>0.16284999999999999</v>
       </c>
       <c r="H88" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -5204,7 +5632,7 @@
         <v>0.16089000000000001</v>
       </c>
       <c r="H89" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -5224,7 +5652,7 @@
         <v>0.16186</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -5247,7 +5675,7 @@
         <v>0.16567999999999999</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -5267,7 +5695,7 @@
         <v>0.16291</v>
       </c>
       <c r="H92" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -5287,7 +5715,7 @@
         <v>0.16320000000000001</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -5307,7 +5735,7 @@
         <v>0.16186</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -5327,7 +5755,7 @@
         <v>0.16184000000000001</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -5350,7 +5778,7 @@
         <v>0.16184000000000001</v>
       </c>
       <c r="H96" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -5373,7 +5801,7 @@
         <v>0.16245999999999999</v>
       </c>
       <c r="H97" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -5396,7 +5824,7 @@
         <v>0.16263</v>
       </c>
       <c r="H98" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -5419,7 +5847,7 @@
         <v>0.16225999999999999</v>
       </c>
       <c r="H99" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.2">
@@ -5442,7 +5870,7 @@
         <v>0.15956999999999999</v>
       </c>
       <c r="H100" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -5465,7 +5893,7 @@
         <v>0.1593</v>
       </c>
       <c r="H101" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.2">
@@ -5488,7 +5916,7 @@
         <v>0.15947</v>
       </c>
       <c r="H102" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.2">
@@ -5511,7 +5939,7 @@
         <v>0.15970999999999999</v>
       </c>
       <c r="H103" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.2">
@@ -5531,7 +5959,7 @@
         <v>0.16849</v>
       </c>
       <c r="H104" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="I104" s="6" t="s">
         <v>70</v>
@@ -5554,7 +5982,7 @@
         <v>0.16799</v>
       </c>
       <c r="H105" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="I105" s="6" t="s">
         <v>71</v>
@@ -5577,7 +6005,7 @@
         <v>0.16767000000000001</v>
       </c>
       <c r="H106" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="I106" s="6" t="s">
         <v>72</v>
@@ -5600,7 +6028,7 @@
         <v>0.1663</v>
       </c>
       <c r="H107" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="I107" s="6" t="s">
         <v>73</v>
@@ -5626,7 +6054,7 @@
         <v>0.16098000000000001</v>
       </c>
       <c r="H108" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.2">
@@ -5649,7 +6077,7 @@
         <v>0.16142999999999999</v>
       </c>
       <c r="H109" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.2">
@@ -5672,7 +6100,7 @@
         <v>0.16142999999999999</v>
       </c>
       <c r="H110" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.2">
@@ -5695,7 +6123,7 @@
         <v>0.15926999999999999</v>
       </c>
       <c r="H111" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.2">
@@ -5718,7 +6146,7 @@
         <v>0.16116</v>
       </c>
       <c r="H112" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -5741,7 +6169,7 @@
         <v>0.16186</v>
       </c>
       <c r="H113" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -5764,7 +6192,7 @@
         <v>0.16450000000000001</v>
       </c>
       <c r="H114" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -5787,7 +6215,7 @@
         <v>0.16012000000000001</v>
       </c>
       <c r="H115" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed why some filtering logs weren't loading properly and moved icp data out of folders to make more sense for reading them in
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/2018_FilteringLog_EDI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carlybauer/Desktop/Reservoirs/Data/DataNotYetUploadedToEDI/Sed_trap/Filtering logs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA95595-E60C-784B-9B75-79D4ACB2DAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F3DB3-2D16-D54B-99D7-B079CABFD9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{05F09711-AF51-DC4E-BE7A-0A95896889C3}"/>
   </bookViews>
@@ -929,10 +929,10 @@
   <dimension ref="A1:M105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A106" sqref="A106:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>

</xml_diff>